<commit_message>
sinusoidal approximation for dial 3 and 4 mapping
</commit_message>
<xml_diff>
--- a/dialmapping.xlsx
+++ b/dialmapping.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,30 +8,67 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/arion_law_mail_utoronto_ca/Documents/SickKids/Continuum_Tool_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{753420D8-6D43-46AD-B0CA-DD7BD5974AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{753420D8-6D43-46AD-B0CA-DD7BD5974AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325F8980-853A-44A2-BC8F-0D7A612FE617}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dialmapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>DiskAngle</t>
   </si>
   <si>
     <t>DeltaCable</t>
   </si>
+  <si>
+    <t>Sinusoid</t>
+  </si>
+  <si>
+    <t>Approximation</t>
+  </si>
+  <si>
+    <t>Vertical Scale</t>
+  </si>
+  <si>
+    <t>Horizontal Scale</t>
+  </si>
+  <si>
+    <t>Vertical Shift</t>
+  </si>
+  <si>
+    <t>Horizontal Shift</t>
+  </si>
+  <si>
+    <t>max delta</t>
+  </si>
+  <si>
+    <t>angle at max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -583,36 +620,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1753,6 +1760,1143 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-74AA-4279-A3AB-D492E392E7F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>dialmapping!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sinusoid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dialmapping!$B$2:$B$182</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="181"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7266459999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7453293000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6179938999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4906584999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3633231000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2359877999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1086524000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9813169999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.8539815999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.7266463000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.5993108999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.104719755</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.113446401</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12217304800000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.13089969400000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.13962633999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.14835298599999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.157079633</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.165806279</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.17453292500000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.18325957100000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.19198621799999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.20071286399999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.20943951</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.218166156</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.226892803</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.23561944900000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.24434609500000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.25307274200000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.26179938800000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.27052603400000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.27925267999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.28797932700000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.29670597300000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.30543261900000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.31415926500000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.322885912</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.331612558</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.34033920400000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.34906585000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.35779249699999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.36651914299999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.375245789</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.383972435</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.39269908199999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.40142572799999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.41015237399999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.41887901999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.42760566700000002</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.43633231300000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.44505895899999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.45378560600000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.46251225200000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.47123889800000002</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.47996554400000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.488692191</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.497418837</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.50614548299999995</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.51487212900000001</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.52359877600000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.53232542199999999</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.54105206800000005</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.549778714</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.55850536100000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.56723200699999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.57595865300000004</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.58468529899999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.59341194600000002</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.60213859199999997</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.61086523800000003</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.61959188399999998</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.62831853100000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.63704517699999996</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.64577182300000002</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.65449846899999997</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.663225116</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.67195176199999995</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.68067840800000001</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.68940505500000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.69813170099999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.70685834700000005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.715584993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.72431164000000003</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.73303828599999998</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.74176493200000004</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.75049157799999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.75921822500000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.76794487099999997</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.77667151700000003</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.78539816299999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.79412481000000001</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.80285145599999996</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.81157810200000002</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.82030474799999997</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.829031395</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.83775804099999995</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.84648468700000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.85521133299999996</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.86393797999999999</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.87266462600000005</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.881391272</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.89011791900000004</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.89884456499999998</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.90757121100000004</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.91629785699999999</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.92502450400000003</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.93375114999999997</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.94247779600000003</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.95120444199999998</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.95993108900000002</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.96865773499999996</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.97738438100000002</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.98611102699999997</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.99483767400000001</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.00356432</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.0122909659999999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.0210176120000001</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.0297442590000001</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.0384709050000001</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.047197551</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.055924197</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.064650844</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.0733774899999999</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.0821041360000001</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.0908307820000001</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.0995574290000001</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.108284075</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.117010721</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1.125737368</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1.134464014</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1.1431906599999999</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1.1519173060000001</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1.1606439529999999</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1.1693705990000001</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1.178097245</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.186823891</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1.195550538</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1.2042771839999999</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1.2130038299999999</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1.2217304760000001</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1.2304571230000001</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.239183769</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.247910415</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1.2566370609999999</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1.265363708</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.2740903539999999</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1.2828170000000001</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.291543646</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1.3002702930000001</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1.308996939</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1.317723585</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1.326450232</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1.335176878</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1.3439035239999999</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1.3526301700000001</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1.3613568170000001</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1.3700834630000001</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1.378810109</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1.387536755</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1.396263402</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1.4049900479999999</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1.4137166940000001</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1.4224433400000001</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1.4311699870000001</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1.439896633</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1.448623279</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.4573499249999999</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1.466076572</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1.4748032179999999</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1.4835298640000001</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1.49225651</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1.5009831570000001</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1.509709803</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1.518436449</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1.5271630949999999</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1.5358897419999999</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1.5446163879999999</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1.5533430340000001</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1.5620696810000001</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1.570796327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dialmapping!$D$2:$D$182</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="181"/>
+                <c:pt idx="0">
+                  <c:v>1.1397810951552678E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9060926296308622E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8678477905770272E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0246315014209166E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3759448788299302E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.9212050294596317E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.6597456106735748E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10590816299005823</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.12713584309104409</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15027133978203722</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.17530467646953696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20222504920674389</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.23102084856490634</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26167965338393628</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29418824272105404</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.32853258644219618</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36469787362441508</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.40266850425549805</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.44242810424052958</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.48395951403708093</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.52724482339273138</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.57226536105094494</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.61900171271205107</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.6674337077905883</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.7175404602483475</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.76930035637750871</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.82269107559213817</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.8776895753990499</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93427213804469122</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.99241436321083842</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0520911577381016</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.1132767864241471</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.1759448566524848</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2400683437810769</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.3056195732433147</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.3725702765720036</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.4408915743672814</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.5105540040774068</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5815275006257985</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.6537814572743357</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.7272847070478865</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.8020055527156509</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.877911746077896</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.954970553248736</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.0331487346654105</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.1124125770633682</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.192727871565574</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.2740599829344621</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.3563738283038478</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.4396339109271956</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.5238042972206398</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.6088486895064058</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.6947304135019525</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.7814124041692181</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.8688572807485304</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.9570273236128939</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.0458845105527117</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.1353904923725677</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.2255066705247724</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.3161941731078635</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.407413892259755</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.4991264591577753</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.5912923237163374</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.68387172989519</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.7768247539430955</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.8701112789735439</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.9636910761768016</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.0575237796082515</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.1515689250187746</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4.2457859241815354</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.3401341470582002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.4345728962412823</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.5290614461033742</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.6235590170520959</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.7180248580837105</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.8124182210557649</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.9066983998851255</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.0008247049086751</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.0947565452548824</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>5.1884534138460578</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.2818748727655009</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.3749806351194316</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.46773053943968</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.5600845883173715</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.6520029233731197</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.7434459059457597</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.834374091812494</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.9247482691326177</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.014529434004408</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.1036788694240576</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.1921581204976643</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.2799290314332605</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.366953721853001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6.4531946634776531</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.5386146560014096</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.6231768628770542</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6.7068447885468503</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6.7895823523236132</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.8713538650947665</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.9521240636538018</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>7.0318580890069278</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>7.1105215569410882</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>7.1880805445410143</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>7.2645015787149454</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.339751703957079</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.4137984608853786</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>7.48660991746618</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>7.5581546495584142</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>7.6284018045281972</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>7.6973210810407107</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>7.7648827582088522</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>7.8310576776038019</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>7.895817302282925</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>7.959133697975135</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>8.0209795599525187</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>8.0813281966313291</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>8.1401535836060344</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>8.1974303463579599</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>8.253133784664497</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>8.3072398579036744</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>8.3597252337216226</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>8.4105672723837372</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>8.459744048553155</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>8.507234338400222</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>8.5530176625676972</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>8.5970742722723728</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>8.6393851683025868</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>8.6799320900215129</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>8.718697552333726</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>8.7556648377656501</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>8.7908179918885949</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>8.8241418556166522</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>8.8556220545946989</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>8.8852450130259193</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>8.912997946163685</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>8.9388688861927879</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>8.9628466736005592</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>8.9849209679118616</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>9.0050822422504151</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>9.0233218026248778</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>9.0396317813425888</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>9.0540051445779568</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>9.0664356890408015</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>9.0769180545341897</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>9.0854477194562655</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>9.0920210051498351</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>9.096635074700675</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>9.0992879386805345</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>9.0999784527680561</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>9.0987063188495689</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>9.0954720859556453</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>9.090277149149653</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>9.0831237483523672</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>9.0740149708454627</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>9.0629547450216723</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>9.0499478417447534</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>9.0349998697601208</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>9.0181172803489602</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>8.9993073542683675</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>8.9785782052400691</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>8.955938772145382</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>8.9313988257645178</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>8.9049689489967605</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>8.8766605424539335</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>8.846485813493457</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>8.814457784996403</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>8.7805902690041506</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>8.7448978743779691</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>8.7073959927458873</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>8.6681008092588989</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>8.6270292698259681</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>8.5841990907868961</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>8.5396287418699419</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>8.4933374588519648</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>8.4453452046178032</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>8.3956726807797111</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>8.3443413077632549</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>8.2913732392841091</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>8.2367913175003871</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>8.1806190799714393</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>8.1228807696447198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4EFE-446D-8848-684FC0032900}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2836,24 +3980,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C182"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2863,8 +4016,18 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <f>$H$2*SIN($H$3*B2 + $H$5)+$H$4</f>
+        <v>1.1397810951552678E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2874,8 +4037,18 @@
       <c r="C3">
         <v>2.4929800000000001E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">$H$2*SIN($H$3*B3 + $H$5)+$H$4</f>
+        <v>1.9060926296308622E-2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2885,8 +4058,18 @@
       <c r="C4">
         <v>9.9984870000000003E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.8678477905770272E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2896,8 +4079,18 @@
       <c r="C5">
         <v>2.2539639E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>4.0246315014209166E-2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2907,8 +4100,12 @@
       <c r="C6">
         <v>4.0116568999999998E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>5.3759448788299302E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2918,8 +4115,19 @@
       <c r="C7">
         <v>6.2705970999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>6.9212050294596317E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <f>MAX(C2:C182)</f>
+        <v>9.0991035369999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2929,8 +4137,18 @@
       <c r="C8">
         <v>9.0261128999999996E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>8.6597456106735748E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2940,8 +4158,19 @@
       <c r="C9">
         <v>0.12271243599999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.10590816299005823</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <f>RADIANS(G8)</f>
+        <v>1.3002702927357754</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2951,8 +4180,12 @@
       <c r="C10">
         <v>0.159968376</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.12713584309104409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2962,8 +4195,12 @@
       <c r="C11">
         <v>0.20191692899999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.15027133978203722</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2973,8 +4210,12 @@
       <c r="C12">
         <v>0.248427336</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.17530467646953696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2984,8 +4225,12 @@
       <c r="C13">
         <v>0.29935214900000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.20222504920674389</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2995,8 +4240,12 @@
       <c r="C14">
         <v>0.35452948499999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.23102084856490634</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3006,8 +4255,12 @@
       <c r="C15">
         <v>0.413785399</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.26167965338393628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3017,8 +4270,12 @@
       <c r="C16">
         <v>0.47693629300000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.29418824272105404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3028,8 +4285,12 @@
       <c r="C17">
         <v>0.54379128399999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.32853258644219618</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3039,8 +4300,12 @@
       <c r="C18">
         <v>0.614154486</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.36469787362441508</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3050,8 +4315,12 @@
       <c r="C19">
         <v>0.68782712300000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0.40266850425549805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3061,8 +4330,12 @@
       <c r="C20">
         <v>0.76460947000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0.44242810424052958</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3072,8 +4345,12 @@
       <c r="C21">
         <v>0.84430258000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.48395951403708093</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3083,8 +4360,12 @@
       <c r="C22">
         <v>0.92670978000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0.52724482339273138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3094,8 +4375,12 @@
       <c r="C23">
         <v>1.0116379499999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.57226536105094494</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3105,8 +4390,12 @@
       <c r="C24">
         <v>1.0988985790000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.61900171271205107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3116,8 +4405,12 @@
       <c r="C25">
         <v>1.1883086110000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0.6674337077905883</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3127,8 +4420,12 @@
       <c r="C26">
         <v>1.279691103</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.7175404602483475</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3138,8 +4435,12 @@
       <c r="C27">
         <v>1.3728757069999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.76930035637750871</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3149,8 +4450,12 @@
       <c r="C28">
         <v>1.4676990000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0.82269107559213817</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3160,8 +4465,12 @@
       <c r="C29">
         <v>1.5640046889999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.8776895753990499</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3171,8 +4480,12 @@
       <c r="C30">
         <v>1.6616436910000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0.93427213804469122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3182,8 +4495,12 @@
       <c r="C31">
         <v>1.7604741349999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0.99241436321083842</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3193,8 +4510,12 @@
       <c r="C32">
         <v>1.860361274</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1.0520911577381016</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3204,8 +4525,12 @@
       <c r="C33">
         <v>1.9611773480000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1.1132767864241471</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3215,8 +4540,12 @@
       <c r="C34">
         <v>2.0628013940000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>1.1759448566524848</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3226,8 +4555,12 @@
       <c r="C35">
         <v>2.1651190169999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1.2400683437810769</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3237,8 +4570,12 @@
       <c r="C36">
         <v>2.2680221459999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1.3056195732433147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3248,8 +4585,12 @@
       <c r="C37">
         <v>2.371408765</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>1.3725702765720036</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3259,8 +4600,12 @@
       <c r="C38">
         <v>2.475182631</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>1.4408915743672814</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3270,8 +4615,12 @@
       <c r="C39">
         <v>2.5792529989999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>1.5105540040774068</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3281,8 +4630,12 @@
       <c r="C40">
         <v>2.6835343360000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>1.5815275006257985</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3292,8 +4645,12 @@
       <c r="C41">
         <v>2.7879460420000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>1.6537814572743357</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3303,8 +4660,12 @@
       <c r="C42">
         <v>2.8924121810000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>1.7272847070478865</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3314,8 +4675,12 @@
       <c r="C43">
         <v>2.9968612120000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>1.8020055527156509</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3325,8 +4690,12 @@
       <c r="C44">
         <v>3.1012257390000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1.877911746077896</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3336,8 +4705,12 @@
       <c r="C45">
         <v>3.2054422659999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>1.954970553248736</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3347,8 +4720,12 @@
       <c r="C46">
         <v>3.3094509639999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>2.0331487346654105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3358,8 +4735,12 @@
       <c r="C47">
         <v>3.4131954489999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>2.1124125770633682</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3369,8 +4750,12 @@
       <c r="C48">
         <v>3.5166225799999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>2.192727871565574</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3380,8 +4765,12 @@
       <c r="C49">
         <v>3.6196822549999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>2.2740599829344621</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3391,8 +4780,12 @@
       <c r="C50">
         <v>3.7223272280000002</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>2.3563738283038478</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3402,8 +4795,12 @@
       <c r="C51">
         <v>3.8245129370000002</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>2.4396339109271956</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3413,8 +4810,12 @@
       <c r="C52">
         <v>3.9261973389999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>2.5238042972206398</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3424,8 +4825,12 @@
       <c r="C53">
         <v>4.0273407580000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>2.6088486895064058</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3435,8 +4840,12 @@
       <c r="C54">
         <v>4.1279057410000002</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>2.6947304135019525</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3446,8 +4855,12 @@
       <c r="C55">
         <v>4.2278569250000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>2.7814124041692181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3457,8 +4870,12 @@
       <c r="C56">
         <v>4.3271609140000002</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>2.8688572807485304</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3468,8 +4885,12 @@
       <c r="C57">
         <v>4.4257861580000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>2.9570273236128939</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3479,8 +4900,12 @@
       <c r="C58">
         <v>4.5237028500000003</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>3.0458845105527117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3490,8 +4915,12 @@
       <c r="C59">
         <v>4.6208828219999996</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>3.1353904923725677</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3501,8 +4930,12 @@
       <c r="C60">
         <v>4.7172994490000004</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>3.2255066705247724</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3512,8 +4945,12 @@
       <c r="C61">
         <v>4.8129275639999998</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>3.3161941731078635</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3523,8 +4960,12 @@
       <c r="C62">
         <v>4.907743376</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>3.407413892259755</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3534,8 +4975,12 @@
       <c r="C63">
         <v>5.0017243899999997</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>3.4991264591577753</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3545,8 +4990,12 @@
       <c r="C64">
         <v>5.0948493399999997</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>3.5912923237163374</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3556,8 +5005,12 @@
       <c r="C65">
         <v>5.187098121</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>3.68387172989519</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3567,8 +5020,12 @@
       <c r="C66">
         <v>5.2784517260000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>3.7768247539430955</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3578,8 +5035,12 @@
       <c r="C67">
         <v>5.3688921890000003</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="1">$H$2*SIN($H$3*B67 + $H$5)+$H$4</f>
+        <v>3.8701112789735439</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3589,8 +5050,12 @@
       <c r="C68">
         <v>5.4584025340000002</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>3.9636910761768016</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3600,8 +5065,12 @@
       <c r="C69">
         <v>5.5469667190000003</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>4.0575237796082515</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3611,8 +5080,12 @@
       <c r="C70">
         <v>5.6345695940000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>4.1515689250187746</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3622,8 +5095,12 @@
       <c r="C71">
         <v>5.7211968549999996</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>4.2457859241815354</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3633,8 +5110,12 @@
       <c r="C72">
         <v>5.8068350009999996</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>4.3401341470582002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3644,8 +5125,12 @@
       <c r="C73">
         <v>5.8914713030000003</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>4.4345728962412823</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3655,8 +5140,12 @@
       <c r="C74">
         <v>5.9750937579999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>4.5290614461033742</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3666,8 +5155,12 @@
       <c r="C75">
         <v>6.0576910650000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>4.6235590170520959</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3677,8 +5170,12 @@
       <c r="C76">
         <v>6.1392525859999996</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>4.7180248580837105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3688,8 +5185,12 @@
       <c r="C77">
         <v>6.21976832</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>4.8124182210557649</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3699,8 +5200,12 @@
       <c r="C78">
         <v>6.2992288780000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>4.9066983998851255</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3710,8 +5215,12 @@
       <c r="C79">
         <v>6.3776254520000002</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>5.0008247049086751</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3721,8 +5230,12 @@
       <c r="C80">
         <v>6.454949794</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>5.0947565452548824</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3732,8 +5245,12 @@
       <c r="C81">
         <v>6.5311941899999999</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>5.1884534138460578</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3743,8 +5260,12 @@
       <c r="C82">
         <v>6.6063514420000002</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>5.2818748727655009</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3754,8 +5275,12 @@
       <c r="C83">
         <v>6.6804148489999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>5.3749806351194316</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3765,8 +5290,12 @@
       <c r="C84">
         <v>6.7533781810000004</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>5.46773053943968</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3776,8 +5305,12 @@
       <c r="C85">
         <v>6.8252356670000003</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>5.5600845883173715</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3787,8 +5320,12 @@
       <c r="C86">
         <v>6.8959819790000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>5.6520029233731197</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3798,8 +5335,12 @@
       <c r="C87">
         <v>6.9656122089999997</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>5.7434459059457597</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3809,8 +5350,12 @@
       <c r="C88">
         <v>7.0341218620000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>5.834374091812494</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3820,8 +5365,12 @@
       <c r="C89">
         <v>7.1015068369999996</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>5.9247482691326177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -3831,8 +5380,12 @@
       <c r="C90">
         <v>7.1677634140000004</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>6.014529434004408</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3842,8 +5395,12 @@
       <c r="C91">
         <v>7.2328882429999997</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>6.1036788694240576</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3853,8 +5410,12 @@
       <c r="C92">
         <v>7.2968783310000003</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>6.1921581204976643</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -3864,8 +5425,12 @@
       <c r="C93">
         <v>7.3597310279999997</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>6.2799290314332605</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -3875,8 +5440,12 @@
       <c r="C94">
         <v>7.42144402</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>6.366953721853001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3886,8 +5455,12 @@
       <c r="C95">
         <v>7.4820153180000002</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>6.4531946634776531</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3897,8 +5470,12 @@
       <c r="C96">
         <v>7.5414432439999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>6.5386146560014096</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -3908,8 +5485,12 @@
       <c r="C97">
         <v>7.5997264270000002</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>6.6231768628770542</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -3919,8 +5500,12 @@
       <c r="C98">
         <v>7.6568637920000002</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>6.7068447885468503</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -3930,8 +5515,12 @@
       <c r="C99">
         <v>7.7128545480000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>6.7895823523236132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -3941,8 +5530,12 @@
       <c r="C100">
         <v>7.7676981850000004</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>6.8713538650947665</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -3952,8 +5545,12 @@
       <c r="C101">
         <v>7.821394465</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>6.9521240636538018</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -3963,8 +5560,12 @@
       <c r="C102">
         <v>7.8739434109999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>7.0318580890069278</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -3974,8 +5575,12 @@
       <c r="C103">
         <v>7.9253453040000004</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>7.1105215569410882</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -3985,8 +5590,12 @@
       <c r="C104">
         <v>7.9756006729999998</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>7.1880805445410143</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -3996,8 +5605,12 @@
       <c r="C105">
         <v>8.0247102909999999</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>7.2645015787149454</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4007,8 +5620,12 @@
       <c r="C106">
         <v>8.0726751659999998</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>7.339751703957079</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4018,8 +5635,12 @@
       <c r="C107">
         <v>8.1194965369999998</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>7.4137984608853786</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4029,8 +5650,12 @@
       <c r="C108">
         <v>8.1651758680000004</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D108">
+        <f t="shared" si="1"/>
+        <v>7.48660991746618</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4040,8 +5665,12 @@
       <c r="C109">
         <v>8.2097148410000003</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D109">
+        <f t="shared" si="1"/>
+        <v>7.5581546495584142</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -4051,8 +5680,12 @@
       <c r="C110">
         <v>8.2531153479999997</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D110">
+        <f t="shared" si="1"/>
+        <v>7.6284018045281972</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -4062,8 +5695,12 @@
       <c r="C111">
         <v>8.2953794940000005</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D111">
+        <f t="shared" si="1"/>
+        <v>7.6973210810407107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -4073,8 +5710,12 @@
       <c r="C112">
         <v>8.3365095819999997</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D112">
+        <f t="shared" si="1"/>
+        <v>7.7648827582088522</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -4084,8 +5725,12 @@
       <c r="C113">
         <v>8.376508115</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D113">
+        <f t="shared" si="1"/>
+        <v>7.8310576776038019</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -4095,8 +5740,12 @@
       <c r="C114">
         <v>8.4153777880000007</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D114">
+        <f t="shared" si="1"/>
+        <v>7.895817302282925</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -4106,8 +5755,12 @@
       <c r="C115">
         <v>8.4531214820000002</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D115">
+        <f t="shared" si="1"/>
+        <v>7.959133697975135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -4117,8 +5770,12 @@
       <c r="C116">
         <v>8.4897422640000002</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D116">
+        <f t="shared" si="1"/>
+        <v>8.0209795599525187</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -4128,8 +5785,12 @@
       <c r="C117">
         <v>8.5252433790000008</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D117">
+        <f t="shared" si="1"/>
+        <v>8.0813281966313291</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -4139,8 +5800,12 @@
       <c r="C118">
         <v>8.5596282450000007</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D118">
+        <f t="shared" si="1"/>
+        <v>8.1401535836060344</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -4150,8 +5815,12 @@
       <c r="C119">
         <v>8.5929004510000002</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D119">
+        <f t="shared" si="1"/>
+        <v>8.1974303463579599</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -4161,8 +5830,12 @@
       <c r="C120">
         <v>8.6250637539999992</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D120">
+        <f t="shared" si="1"/>
+        <v>8.253133784664497</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -4172,8 +5845,12 @@
       <c r="C121">
         <v>8.6561220690000003</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D121">
+        <f t="shared" si="1"/>
+        <v>8.3072398579036744</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -4183,8 +5860,12 @@
       <c r="C122">
         <v>8.6860794729999995</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D122">
+        <f t="shared" si="1"/>
+        <v>8.3597252337216226</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -4194,8 +5875,12 @@
       <c r="C123">
         <v>8.7149401950000005</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D123">
+        <f t="shared" si="1"/>
+        <v>8.4105672723837372</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -4205,8 +5890,12 @@
       <c r="C124">
         <v>8.7427086149999997</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D124">
+        <f t="shared" si="1"/>
+        <v>8.459744048553155</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -4216,8 +5905,12 @@
       <c r="C125">
         <v>8.7693892590000004</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D125">
+        <f t="shared" si="1"/>
+        <v>8.507234338400222</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -4227,8 +5920,12 @@
       <c r="C126">
         <v>8.794986797</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D126">
+        <f t="shared" si="1"/>
+        <v>8.5530176625676972</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -4238,8 +5935,12 @@
       <c r="C127">
         <v>8.8195060380000001</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D127">
+        <f t="shared" si="1"/>
+        <v>8.5970742722723728</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -4249,8 +5950,12 @@
       <c r="C128">
         <v>8.8429519259999996</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D128">
+        <f t="shared" si="1"/>
+        <v>8.6393851683025868</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -4260,8 +5965,12 @@
       <c r="C129">
         <v>8.8653295389999993</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D129">
+        <f t="shared" si="1"/>
+        <v>8.6799320900215129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -4271,8 +5980,12 @@
       <c r="C130">
         <v>8.8866440840000003</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D130">
+        <f t="shared" si="1"/>
+        <v>8.718697552333726</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -4282,8 +5995,12 @@
       <c r="C131">
         <v>8.9069008929999995</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D131">
+        <f t="shared" ref="D131:D182" si="2">$H$2*SIN($H$3*B131 + $H$5)+$H$4</f>
+        <v>8.7556648377656501</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -4293,8 +6010,12 @@
       <c r="C132">
         <v>8.9261054200000007</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D132">
+        <f t="shared" si="2"/>
+        <v>8.7908179918885949</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -4304,8 +6025,12 @@
       <c r="C133">
         <v>8.9442632389999996</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D133">
+        <f t="shared" si="2"/>
+        <v>8.8241418556166522</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -4315,8 +6040,12 @@
       <c r="C134">
         <v>8.9613800399999999</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D134">
+        <f t="shared" si="2"/>
+        <v>8.8556220545946989</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -4326,8 +6055,12 @@
       <c r="C135">
         <v>8.9774616260000002</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D135">
+        <f t="shared" si="2"/>
+        <v>8.8852450130259193</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -4337,8 +6070,12 @@
       <c r="C136">
         <v>8.9925139099999996</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D136">
+        <f t="shared" si="2"/>
+        <v>8.912997946163685</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -4348,8 +6085,12 @@
       <c r="C137">
         <v>9.0065429090000002</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D137">
+        <f t="shared" si="2"/>
+        <v>8.9388688861927879</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -4359,8 +6100,12 @@
       <c r="C138">
         <v>9.0195547479999991</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D138">
+        <f t="shared" si="2"/>
+        <v>8.9628466736005592</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -4370,8 +6115,12 @@
       <c r="C139">
         <v>9.0315556499999996</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D139">
+        <f t="shared" si="2"/>
+        <v>8.9849209679118616</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -4381,8 +6130,12 @@
       <c r="C140">
         <v>9.0425519360000006</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D140">
+        <f t="shared" si="2"/>
+        <v>9.0050822422504151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -4392,8 +6145,12 @@
       <c r="C141">
         <v>9.0525500220000001</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D141">
+        <f t="shared" si="2"/>
+        <v>9.0233218026248778</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -4403,8 +6160,12 @@
       <c r="C142">
         <v>9.0615564160000002</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D142">
+        <f t="shared" si="2"/>
+        <v>9.0396317813425888</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -4414,8 +6175,12 @@
       <c r="C143">
         <v>9.0695777149999994</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D143">
+        <f t="shared" si="2"/>
+        <v>9.0540051445779568</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
@@ -4425,8 +6190,12 @@
       <c r="C144">
         <v>9.0766206020000002</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D144">
+        <f t="shared" si="2"/>
+        <v>9.0664356890408015</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -4436,8 +6205,12 @@
       <c r="C145">
         <v>9.0826918449999994</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D145">
+        <f t="shared" si="2"/>
+        <v>9.0769180545341897</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
@@ -4447,8 +6220,12 @@
       <c r="C146">
         <v>9.0877982910000004</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D146">
+        <f t="shared" si="2"/>
+        <v>9.0854477194562655</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -4458,8 +6235,12 @@
       <c r="C147">
         <v>9.0919468650000006</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D147">
+        <f t="shared" si="2"/>
+        <v>9.0920210051498351</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
@@ -4469,8 +6250,12 @@
       <c r="C148">
         <v>9.0951445690000003</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D148">
+        <f t="shared" si="2"/>
+        <v>9.096635074700675</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -4480,8 +6265,12 @@
       <c r="C149">
         <v>9.0973984750000003</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D149">
+        <f t="shared" si="2"/>
+        <v>9.0992879386805345</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
@@ -4491,8 +6280,12 @@
       <c r="C150">
         <v>9.0987157270000001</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D150">
+        <f t="shared" si="2"/>
+        <v>9.0999784527680561</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -4502,8 +6295,16 @@
       <c r="C151">
         <v>9.0991035369999995</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D151">
+        <f t="shared" si="2"/>
+        <v>9.0987063188495689</v>
+      </c>
+      <c r="E151">
+        <f>DEGREES(B151)</f>
+        <v>74.500000015138951</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
@@ -4513,8 +6314,12 @@
       <c r="C152">
         <v>9.0985691800000001</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D152">
+        <f t="shared" si="2"/>
+        <v>9.0954720859556453</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -4524,8 +6329,12 @@
       <c r="C153">
         <v>9.0971199949999999</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D153">
+        <f t="shared" si="2"/>
+        <v>9.090277149149653</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
@@ -4535,8 +6344,12 @@
       <c r="C154">
         <v>9.0947633779999997</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D154">
+        <f t="shared" si="2"/>
+        <v>9.0831237483523672</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -4546,8 +6359,12 @@
       <c r="C155">
         <v>9.0915067860000001</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D155">
+        <f t="shared" si="2"/>
+        <v>9.0740149708454627</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
@@ -4557,8 +6374,12 @@
       <c r="C156">
         <v>9.0873577280000006</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D156">
+        <f t="shared" si="2"/>
+        <v>9.0629547450216723</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -4568,8 +6389,12 @@
       <c r="C157">
         <v>9.0823237670000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D157">
+        <f t="shared" si="2"/>
+        <v>9.0499478417447534</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
@@ -4579,8 +6404,12 @@
       <c r="C158">
         <v>9.0764125159999995</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D158">
+        <f t="shared" si="2"/>
+        <v>9.0349998697601208</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -4590,8 +6419,12 @@
       <c r="C159">
         <v>9.0696316350000004</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D159">
+        <f t="shared" si="2"/>
+        <v>9.0181172803489602</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
@@ -4601,8 +6434,12 @@
       <c r="C160">
         <v>9.0619888290000006</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D160">
+        <f t="shared" si="2"/>
+        <v>8.9993073542683675</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -4612,8 +6449,12 @@
       <c r="C161">
         <v>9.053491846</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D161">
+        <f t="shared" si="2"/>
+        <v>8.9785782052400691</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
@@ -4623,8 +6464,12 @@
       <c r="C162">
         <v>9.0441484780000003</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D162">
+        <f t="shared" si="2"/>
+        <v>8.955938772145382</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -4634,8 +6479,12 @@
       <c r="C163">
         <v>9.0339665500000006</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D163">
+        <f t="shared" si="2"/>
+        <v>8.9313988257645178</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -4645,8 +6494,12 @@
       <c r="C164">
         <v>9.0229539269999997</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D164">
+        <f t="shared" si="2"/>
+        <v>8.9049689489967605</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -4656,8 +6509,12 @@
       <c r="C165">
         <v>9.0111185089999992</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D165">
+        <f t="shared" si="2"/>
+        <v>8.8766605424539335</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
@@ -4667,8 +6524,12 @@
       <c r="C166">
         <v>8.9984682239999998</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D166">
+        <f t="shared" si="2"/>
+        <v>8.846485813493457</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -4678,8 +6539,12 @@
       <c r="C167">
         <v>8.9850110339999993</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D167">
+        <f t="shared" si="2"/>
+        <v>8.814457784996403</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
@@ -4689,8 +6554,12 @@
       <c r="C168">
         <v>8.9707549259999997</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D168">
+        <f t="shared" si="2"/>
+        <v>8.7805902690041506</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -4700,8 +6569,12 @@
       <c r="C169">
         <v>8.9557079149999996</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D169">
+        <f t="shared" si="2"/>
+        <v>8.7448978743779691</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
@@ -4711,8 +6584,12 @@
       <c r="C170">
         <v>8.9398780379999998</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D170">
+        <f t="shared" si="2"/>
+        <v>8.7073959927458873</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -4722,8 +6599,12 @@
       <c r="C171">
         <v>8.9232733549999992</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D171">
+        <f t="shared" si="2"/>
+        <v>8.6681008092588989</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
@@ -4733,8 +6614,12 @@
       <c r="C172">
         <v>8.9059019450000001</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D172">
+        <f t="shared" si="2"/>
+        <v>8.6270292698259681</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -4744,8 +6629,12 @@
       <c r="C173">
         <v>8.8877719059999993</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D173">
+        <f t="shared" si="2"/>
+        <v>8.5841990907868961</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
@@ -4755,8 +6644,12 @@
       <c r="C174">
         <v>8.8688913520000003</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D174">
+        <f t="shared" si="2"/>
+        <v>8.5396287418699419</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -4766,8 +6659,12 @@
       <c r="C175">
         <v>8.8492684110000006</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D175">
+        <f t="shared" si="2"/>
+        <v>8.4933374588519648</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
@@ -4777,8 +6674,12 @@
       <c r="C176">
         <v>8.8289112250000006</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D176">
+        <f t="shared" si="2"/>
+        <v>8.4453452046178032</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -4788,8 +6689,12 @@
       <c r="C177">
         <v>8.8078279439999996</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D177">
+        <f t="shared" si="2"/>
+        <v>8.3956726807797111</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
@@ -4799,8 +6704,12 @@
       <c r="C178">
         <v>8.7860267309999998</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D178">
+        <f t="shared" si="2"/>
+        <v>8.3443413077632549</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -4810,8 +6719,12 @@
       <c r="C179">
         <v>8.7635157540000002</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D179">
+        <f t="shared" si="2"/>
+        <v>8.2913732392841091</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
@@ -4821,8 +6734,12 @@
       <c r="C180">
         <v>8.7403031880000004</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D180">
+        <f t="shared" si="2"/>
+        <v>8.2367913175003871</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -4832,8 +6749,12 @@
       <c r="C181">
         <v>8.7163972140000006</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D181">
+        <f t="shared" si="2"/>
+        <v>8.1806190799714393</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
@@ -4842,6 +6763,10 @@
       </c>
       <c r="C182">
         <v>8.6918060130000008</v>
+      </c>
+      <c r="D182">
+        <f t="shared" si="2"/>
+        <v>8.1228807696447198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resolved numerical IK arccos NaN issue due to floating point error trace calculation
</commit_message>
<xml_diff>
--- a/dialmapping.xlsx
+++ b/dialmapping.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/arion_law_mail_utoronto_ca/Documents/SickKids/Continuum_Tool_Modeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arion Law\OneDrive - University of Toronto\SickKids\Continuum_Tool_Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{753420D8-6D43-46AD-B0CA-DD7BD5974AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{325F8980-853A-44A2-BC8F-0D7A612FE617}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="dialmapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,7 +621,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13355261856126077"/>
+          <c:y val="4.8245614035087717E-2"/>
+          <c:w val="0.82189407033655149"/>
+          <c:h val="0.75700303909379751"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -2932,6 +2941,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Dial Angle</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2994,6 +3059,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Cable Displacement</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3043,8 +3164,41 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3052,7 +3206,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3647,16 +3800,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>6724</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>179574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>27174</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3980,11 +4133,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated xlsx with visualized mappings
</commit_message>
<xml_diff>
--- a/dialmapping.xlsx
+++ b/dialmapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/arion_law_mail_utoronto_ca/Documents/SickKids/Continuum_Tool_Modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_EDDBD729D2DF9199826D7835419AFF831612B8A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66FD8B72-BBDA-4CF5-B6D4-78E918B39839}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_EDDBD729D2DF9199826D7835419AFF831612B8A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B81531BD-F98C-4866-BFBC-44F87EB094F4}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dialmapping" sheetId="1" r:id="rId1"/>
@@ -2361,544 +2361,544 @@
                   <c:v>1.1397810951552678E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9060926296308622E-2</c:v>
+                  <c:v>1.4065603567027019E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8678477905770272E-2</c:v>
+                  <c:v>1.7013194319355662E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0246315014209166E-2</c:v>
+                  <c:v>2.0240400711730722E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.3759448788299302E-2</c:v>
+                  <c:v>2.3747023996616434E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.9212050294596317E-2</c:v>
+                  <c:v>2.7532847868981136E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.6597456106735748E-2</c:v>
+                  <c:v>3.1597639283155843E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10590816299005823</c:v>
+                  <c:v>3.5941146572097793E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12713584309104409</c:v>
+                  <c:v>4.0563102257643813E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15027133978203722</c:v>
+                  <c:v>4.5463221235813478E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.17530467646953696</c:v>
+                  <c:v>5.0641201853466988E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20222504920674389</c:v>
+                  <c:v>5.6096723521687153E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.23102084856490634</c:v>
+                  <c:v>6.1829450295658894E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.26167965338393628</c:v>
+                  <c:v>6.7839028553811964E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.29418824272105404</c:v>
+                  <c:v>7.4125088333230948E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.32853258644219618</c:v>
+                  <c:v>8.0687240439508479E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.36469787362441508</c:v>
+                  <c:v>8.7525080792714149E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.40266850425549805</c:v>
+                  <c:v>9.4638187602667401E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.44242810424052958</c:v>
+                  <c:v>0.1020261229617887</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.48395951403708093</c:v>
+                  <c:v>0.10968842945426882</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.52724482339273138</c:v>
+                  <c:v>0.11762463526383549</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.57226536105094494</c:v>
+                  <c:v>0.12583425084796218</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.61900171271205107</c:v>
+                  <c:v>0.13431677078655913</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.6674337077905883</c:v>
+                  <c:v>0.14307166989383191</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.7175404602483475</c:v>
+                  <c:v>0.15209840908279482</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.76930035637750871</c:v>
+                  <c:v>0.16139643154168759</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.82269107559213817</c:v>
+                  <c:v>0.17096516483670765</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.8776895753990499</c:v>
+                  <c:v>0.18080401653036571</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.93427213804469122</c:v>
+                  <c:v>0.19091238079697614</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99241436321083842</c:v>
+                  <c:v>0.20128963530958366</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0520911577381016</c:v>
+                  <c:v>0.21193513757200488</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.1132767864241471</c:v>
+                  <c:v>0.22284823209330717</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.1759448566524848</c:v>
+                  <c:v>0.23402824570245517</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.2400683437810769</c:v>
+                  <c:v>0.24547449009045863</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.3056195732433147</c:v>
+                  <c:v>0.25718625657581651</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.3725702765720036</c:v>
+                  <c:v>0.26916282401804992</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.4408915743672814</c:v>
+                  <c:v>0.2814034536461083</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.5105540040774068</c:v>
+                  <c:v>0.29390739184824533</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.5815275006257985</c:v>
+                  <c:v>0.30667386445702327</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.6537814572743357</c:v>
+                  <c:v>0.3197020853940975</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.7272847070478865</c:v>
+                  <c:v>0.33299125101747951</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.8020055527156509</c:v>
+                  <c:v>0.34654054315639193</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.877911746077896</c:v>
+                  <c:v>0.36034912292146881</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.954970553248736</c:v>
+                  <c:v>0.37441614007226498</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.0331487346654105</c:v>
+                  <c:v>0.38874072688895023</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.1124125770633682</c:v>
+                  <c:v>0.40332200144915209</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.192727871565574</c:v>
+                  <c:v>0.41815906096946254</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.2740599829344621</c:v>
+                  <c:v>0.43325099188641492</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.3563738283038478</c:v>
+                  <c:v>0.4485968632586772</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.4396339109271956</c:v>
+                  <c:v>0.46419573028263006</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.5238042972206398</c:v>
+                  <c:v>0.48004662717175872</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.6088486895064058</c:v>
+                  <c:v>0.49614857794115785</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.6947304135019525</c:v>
+                  <c:v>0.51250059123480796</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.7814124041692181</c:v>
+                  <c:v>0.52910165463597725</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.8688572807485304</c:v>
+                  <c:v>0.54595074597243354</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.9570273236128939</c:v>
+                  <c:v>0.56304682591291844</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.0458845105527117</c:v>
+                  <c:v>0.58038884189205264</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.1353904923725677</c:v>
+                  <c:v>0.59797572019819034</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3.2255066705247724</c:v>
+                  <c:v>0.61580637796307824</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.3161941731078635</c:v>
+                  <c:v>0.63387971530782083</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.407413892259755</c:v>
+                  <c:v>0.65219461949643476</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3.4991264591577753</c:v>
+                  <c:v>0.67074995658198189</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.5912923237163374</c:v>
+                  <c:v>0.689544584068849</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.68387172989519</c:v>
+                  <c:v>0.70857734261595162</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3.7768247539430955</c:v>
+                  <c:v>0.72784706041483771</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3.8701112789735439</c:v>
+                  <c:v>0.74735254440234478</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.9636910761768016</c:v>
+                  <c:v>0.76709259358300752</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.0575237796082515</c:v>
+                  <c:v>0.7870659902976791</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.1515689250187746</c:v>
+                  <c:v>0.8072715048218746</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4.2457859241815354</c:v>
+                  <c:v>0.82770788615361646</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4.3401341470582002</c:v>
+                  <c:v>0.84837387598282232</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.4345728962412823</c:v>
+                  <c:v>0.86926819953396794</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.5290614461033742</c:v>
+                  <c:v>0.89038957038012434</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.6235590170520959</c:v>
+                  <c:v>0.91173668081508685</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.7180248580837105</c:v>
+                  <c:v>0.93330821645595607</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.8124182210557649</c:v>
+                  <c:v>0.95510284666888134</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.9066983998851255</c:v>
+                  <c:v>0.97711922959403452</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5.0008247049086751</c:v>
+                  <c:v>0.99935600211153419</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.0947565452548824</c:v>
+                  <c:v>1.021811795062801</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.1884534138460578</c:v>
+                  <c:v>1.0444852258794319</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5.2818748727655009</c:v>
+                  <c:v>1.0673748907611547</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5.3749806351194316</c:v>
+                  <c:v>1.0904793803514456</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5.46773053943968</c:v>
+                  <c:v>1.1137972694566387</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5.5600845883173715</c:v>
+                  <c:v>1.1373271224279948</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.6520029233731197</c:v>
+                  <c:v>1.1610674824408158</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5.7434459059457597</c:v>
+                  <c:v>1.1850168877621621</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>5.834374091812494</c:v>
+                  <c:v>1.2091738610799903</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>5.9247482691326177</c:v>
+                  <c:v>1.2335369150820346</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6.014529434004408</c:v>
+                  <c:v>1.2581045413568828</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6.1036788694240576</c:v>
+                  <c:v>1.2828752272377346</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>6.1921581204976643</c:v>
+                  <c:v>1.3078474447520936</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6.2799290314332605</c:v>
+                  <c:v>1.333019656391969</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>6.366953721853001</c:v>
+                  <c:v>1.3583903036478522</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>6.4531946634776531</c:v>
+                  <c:v>1.3839578244119006</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>6.5386146560014096</c:v>
+                  <c:v>1.4097206415590935</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>6.6231768628770542</c:v>
+                  <c:v>1.4356771689030463</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>6.7068447885468503</c:v>
+                  <c:v>1.461825799374215</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>6.7895823523236132</c:v>
+                  <c:v>1.4881649229653284</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>6.8713538650947665</c:v>
+                  <c:v>1.5146929149552708</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>6.9521240636538018</c:v>
+                  <c:v>1.5414081420446406</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.0318580890069278</c:v>
+                  <c:v>1.568308950189842</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>7.1105215569410882</c:v>
+                  <c:v>1.5953936830730564</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>7.1880805445410143</c:v>
+                  <c:v>1.6226606731154223</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>7.2645015787149454</c:v>
+                  <c:v>1.6501082321115557</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>7.339751703957079</c:v>
+                  <c:v>1.6777346700809845</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>7.4137984608853786</c:v>
+                  <c:v>1.7055382828949837</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>7.48660991746618</c:v>
+                  <c:v>1.7335173587120041</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>7.5581546495584142</c:v>
+                  <c:v>1.7616701652386606</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>7.6284018045281972</c:v>
+                  <c:v>1.7899949690734838</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>7.6973210810407107</c:v>
+                  <c:v>1.8184900230092547</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>7.7648827582088522</c:v>
+                  <c:v>1.8471535726311155</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>7.8310576776038019</c:v>
+                  <c:v>1.8759838432672455</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>7.895817302282925</c:v>
+                  <c:v>1.9049790598058371</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>7.959133697975135</c:v>
+                  <c:v>1.9341374336854593</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>8.0209795599525187</c:v>
+                  <c:v>1.9634571696493408</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>8.0813281966313291</c:v>
+                  <c:v>1.9929364523986131</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>8.1401535836060344</c:v>
+                  <c:v>2.0225734668629491</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>8.1974303463579599</c:v>
+                  <c:v>2.0523663848918021</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>8.253133784664497</c:v>
+                  <c:v>2.0823133721581892</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>8.3072398579036744</c:v>
+                  <c:v>2.1124125745276738</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>8.3597252337216226</c:v>
+                  <c:v>2.1426621387626645</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>8.4105672723837372</c:v>
+                  <c:v>2.1730601989276632</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>8.459744048553155</c:v>
+                  <c:v>2.2036048834357342</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>8.507234338400222</c:v>
+                  <c:v>2.2342943011466811</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>8.5530176625676972</c:v>
+                  <c:v>2.2651265624845713</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>8.5970742722723728</c:v>
+                  <c:v>2.2960997655704034</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>8.6393851683025868</c:v>
+                  <c:v>2.3272120034043224</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>8.6799320900215129</c:v>
+                  <c:v>2.358461349706698</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>8.718697552333726</c:v>
+                  <c:v>2.3898458804280378</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>8.7556648377656501</c:v>
+                  <c:v>2.4213636632420013</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>8.7908179918885949</c:v>
+                  <c:v>2.4530127467600895</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>8.8241418556166522</c:v>
+                  <c:v>2.4847911823219433</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>8.8556220545946989</c:v>
+                  <c:v>2.5166970096840848</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>8.8852450130259193</c:v>
+                  <c:v>2.548728264422528</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>8.912997946163685</c:v>
+                  <c:v>2.5808829633577379</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>8.9388688861927879</c:v>
+                  <c:v>2.6131591266998981</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>8.9628466736005592</c:v>
+                  <c:v>2.6455547635033416</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>8.9849209679118616</c:v>
+                  <c:v>2.678067879185094</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>9.0050822422504151</c:v>
+                  <c:v>2.7106964607317288</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>9.0233218026248778</c:v>
+                  <c:v>2.7434384991777998</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>9.0396317813425888</c:v>
+                  <c:v>2.7762919748402668</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>9.0540051445779568</c:v>
+                  <c:v>2.8092548649455775</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>9.0664356890408015</c:v>
+                  <c:v>2.8423251286330231</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>9.0769180545341897</c:v>
+                  <c:v>2.8755007297441257</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>9.0854477194562655</c:v>
+                  <c:v>2.9087796218516599</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>9.0920210051498351</c:v>
+                  <c:v>2.9421597559877268</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>9.096635074700675</c:v>
+                  <c:v>2.9756390654584197</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>9.0992879386805345</c:v>
+                  <c:v>3.0092154889216713</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>9.0999784527680561</c:v>
+                  <c:v>3.0428869552256463</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>9.0987063188495689</c:v>
+                  <c:v>3.0766513912301869</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>9.0954720859556453</c:v>
+                  <c:v>3.1105067064477594</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>9.090277149149653</c:v>
+                  <c:v>3.1444508163870077</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>9.0831237483523672</c:v>
+                  <c:v>3.1784816311199942</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>9.0740149708454627</c:v>
+                  <c:v>3.2125970436666447</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>9.0629547450216723</c:v>
+                  <c:v>3.2467949535224574</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>9.0499478417447534</c:v>
+                  <c:v>3.2810732511993912</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>9.0349998697601208</c:v>
+                  <c:v>3.3154298261920832</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>9.0181172803489602</c:v>
+                  <c:v>3.3498625513513729</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>8.9993073542683675</c:v>
+                  <c:v>3.3843693066372378</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>8.9785782052400691</c:v>
+                  <c:v>3.418947963510595</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>8.955938772145382</c:v>
+                  <c:v>3.4535963929714715</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>8.9313988257645178</c:v>
+                  <c:v>3.4883124498008606</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>8.9049689489967605</c:v>
+                  <c:v>3.5230939965154393</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>8.8766605424539335</c:v>
+                  <c:v>3.5579388876256979</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>8.846485813493457</c:v>
+                  <c:v>3.5928449777381131</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>8.814457784996403</c:v>
+                  <c:v>3.6278101056809096</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>8.7805902690041506</c:v>
+                  <c:v>3.6628321186369002</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>8.7448978743779691</c:v>
+                  <c:v>3.6979088562834859</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>8.7073959927458873</c:v>
+                  <c:v>3.7330381589508428</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>8.6681008092588989</c:v>
+                  <c:v>3.7682178516472353</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>8.6270292698259681</c:v>
+                  <c:v>3.8034457683461893</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>8.5841990907868961</c:v>
+                  <c:v>3.8387197360239904</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>8.5396287418699419</c:v>
+                  <c:v>3.8740375828658475</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>8.4933374588519648</c:v>
+                  <c:v>3.9093971222065216</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>8.4453452046178032</c:v>
+                  <c:v>3.9447961769478512</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>8.3956726807797111</c:v>
+                  <c:v>3.9802325635095284</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>8.3443413077632549</c:v>
+                  <c:v>4.0157041000751068</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>8.2913732392841091</c:v>
+                  <c:v>4.0512085904638209</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>8.2367913175003871</c:v>
+                  <c:v>4.0867438486543604</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>8.1806190799714393</c:v>
+                  <c:v>4.1223076867416104</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>8.1228807696447198</c:v>
+                  <c:v>4.1578979028300624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4132,18 +4132,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H182"/>
+  <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4157,8 +4157,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
+        <f>DEGREES(B2)</f>
         <v>0</v>
       </c>
       <c r="B2">
@@ -4177,10 +4178,15 @@
       <c r="H2">
         <v>4.55</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f>0.66*3</f>
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>1</v>
+        <f t="shared" ref="A3:A66" si="0">DEGREES(B3)</f>
+        <v>0.49999998510472177</v>
       </c>
       <c r="B3">
         <v>8.7266459999999994E-3</v>
@@ -4189,19 +4195,20 @@
         <v>2.4929800000000001E-3</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="0">$H$2*SIN($H$3*B3 + $H$5)+$H$4</f>
-        <v>1.9060926296308622E-2</v>
+        <f t="shared" ref="D3:D66" si="1">$H$2*SIN($H$3*B3 + $H$5)+$H$4</f>
+        <v>1.4065603567027019E-2</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="H3">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1.0000000275052232</v>
       </c>
       <c r="B4">
         <v>1.7453293000000002E-2</v>
@@ -4210,8 +4217,8 @@
         <v>9.9984870000000003E-3</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
-        <v>2.8678477905770272E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.7013194319355662E-2</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -4220,9 +4227,10 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>1.5000000126099449</v>
       </c>
       <c r="B5">
         <v>2.6179938999999999E-2</v>
@@ -4231,8 +4239,8 @@
         <v>2.2539639E-2</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>4.0246315014209166E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.0240400711730722E-2</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -4241,9 +4249,10 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>1.9999999977146665</v>
       </c>
       <c r="B6">
         <v>3.4906584999999997E-2</v>
@@ -4252,13 +4261,14 @@
         <v>4.0116568999999998E-2</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.3747023996616434E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7">
         <f t="shared" si="0"/>
-        <v>5.3759448788299302E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
+        <v>2.4999999828193884</v>
       </c>
       <c r="B7">
         <v>4.3633231000000001E-2</v>
@@ -4267,8 +4277,8 @@
         <v>6.2705970999999999E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>6.9212050294596317E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.7532847868981136E-2</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -4278,9 +4288,10 @@
         <v>9.0991035369999995</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>3.0000000252198897</v>
       </c>
       <c r="B8">
         <v>5.2359877999999999E-2</v>
@@ -4289,8 +4300,8 @@
         <v>9.0261128999999996E-2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>8.6597456106735748E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.1597639283155843E-2</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -4299,9 +4310,10 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>3.5000000103246118</v>
       </c>
       <c r="B9">
         <v>6.1086524000000003E-2</v>
@@ -4310,8 +4322,8 @@
         <v>0.12271243599999999</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.10590816299005823</v>
+        <f t="shared" si="1"/>
+        <v>3.5941146572097793E-2</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -4321,9 +4333,10 @@
         <v>1.3002702927357754</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>3.999999995429333</v>
       </c>
       <c r="B10">
         <v>6.9813169999999994E-2</v>
@@ -4332,13 +4345,14 @@
         <v>0.159968376</v>
       </c>
       <c r="D10">
+        <f t="shared" si="1"/>
+        <v>4.0563102257643813E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11">
         <f t="shared" si="0"/>
-        <v>0.12713584309104409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
+        <v>4.4999999805340547</v>
       </c>
       <c r="B11">
         <v>7.8539815999999998E-2</v>
@@ -4347,13 +4361,14 @@
         <v>0.20191692899999999</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>4.5463221235813478E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12">
         <f t="shared" si="0"/>
-        <v>0.15027133978203722</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
+        <v>5.0000000229345565</v>
       </c>
       <c r="B12">
         <v>8.7266463000000002E-2</v>
@@ -4362,13 +4377,14 @@
         <v>0.248427336</v>
       </c>
       <c r="D12">
+        <f t="shared" si="1"/>
+        <v>5.0641201853466988E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13">
         <f t="shared" si="0"/>
-        <v>0.17530467646953696</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
+        <v>5.5000000080392777</v>
       </c>
       <c r="B13">
         <v>9.5993108999999993E-2</v>
@@ -4377,13 +4393,14 @@
         <v>0.29935214900000001</v>
       </c>
       <c r="D13">
+        <f t="shared" si="1"/>
+        <v>5.6096723521687153E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14">
         <f t="shared" si="0"/>
-        <v>0.20222504920674389</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
+        <v>5.9999999931439998</v>
       </c>
       <c r="B14">
         <v>0.104719755</v>
@@ -4392,13 +4409,14 @@
         <v>0.35452948499999998</v>
       </c>
       <c r="D14">
+        <f t="shared" si="1"/>
+        <v>6.1829450295658894E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15">
         <f t="shared" si="0"/>
-        <v>0.23102084856490634</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
+        <v>6.4999999782487219</v>
       </c>
       <c r="B15">
         <v>0.113446401</v>
@@ -4407,13 +4425,14 @@
         <v>0.413785399</v>
       </c>
       <c r="D15">
+        <f t="shared" si="1"/>
+        <v>6.7839028553811964E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16">
         <f t="shared" si="0"/>
-        <v>0.26167965338393628</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
+        <v>7.0000000206492237</v>
       </c>
       <c r="B16">
         <v>0.12217304800000001</v>
@@ -4422,13 +4441,14 @@
         <v>0.47693629300000001</v>
       </c>
       <c r="D16">
+        <f t="shared" si="1"/>
+        <v>7.4125088333230948E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17">
         <f t="shared" si="0"/>
-        <v>0.29418824272105404</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
+        <v>7.5000000057539458</v>
       </c>
       <c r="B17">
         <v>0.13089969400000001</v>
@@ -4437,13 +4457,14 @@
         <v>0.54379128399999999</v>
       </c>
       <c r="D17">
+        <f t="shared" si="1"/>
+        <v>8.0687240439508479E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18">
         <f t="shared" si="0"/>
-        <v>0.32853258644219618</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
+        <v>7.9999999908586661</v>
       </c>
       <c r="B18">
         <v>0.13962633999999999</v>
@@ -4452,13 +4473,14 @@
         <v>0.614154486</v>
       </c>
       <c r="D18">
+        <f t="shared" si="1"/>
+        <v>8.7525080792714149E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19">
         <f t="shared" si="0"/>
-        <v>0.36469787362441508</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
+        <v>8.4999999759633891</v>
       </c>
       <c r="B19">
         <v>0.14835298599999999</v>
@@ -4467,13 +4489,14 @@
         <v>0.68782712300000004</v>
       </c>
       <c r="D19">
+        <f t="shared" si="1"/>
+        <v>9.4638187602667401E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20">
         <f t="shared" si="0"/>
-        <v>0.40266850425549805</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
+        <v>9.00000001836389</v>
       </c>
       <c r="B20">
         <v>0.157079633</v>
@@ -4482,13 +4505,14 @@
         <v>0.76460947000000001</v>
       </c>
       <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0.1020261229617887</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21">
         <f t="shared" si="0"/>
-        <v>0.44242810424052958</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
+        <v>9.5000000034686121</v>
       </c>
       <c r="B21">
         <v>0.165806279</v>
@@ -4497,13 +4521,14 @@
         <v>0.84430258000000002</v>
       </c>
       <c r="D21">
+        <f t="shared" si="1"/>
+        <v>0.10968842945426882</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22">
         <f t="shared" si="0"/>
-        <v>0.48395951403708093</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
+        <v>9.9999999885733342</v>
       </c>
       <c r="B22">
         <v>0.17453292500000001</v>
@@ -4512,13 +4537,14 @@
         <v>0.92670978000000004</v>
       </c>
       <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0.11762463526383549</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23">
         <f t="shared" si="0"/>
-        <v>0.52724482339273138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
+        <v>10.499999973678056</v>
       </c>
       <c r="B23">
         <v>0.18325957100000001</v>
@@ -4527,13 +4553,14 @@
         <v>1.0116379499999999</v>
       </c>
       <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0.12583425084796218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24">
         <f t="shared" si="0"/>
-        <v>0.57226536105094494</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
+        <v>11.000000016078555</v>
       </c>
       <c r="B24">
         <v>0.19198621799999999</v>
@@ -4542,13 +4569,14 @@
         <v>1.0988985790000001</v>
       </c>
       <c r="D24">
+        <f t="shared" si="1"/>
+        <v>0.13431677078655913</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25">
         <f t="shared" si="0"/>
-        <v>0.61900171271205107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
+        <v>11.500000001183277</v>
       </c>
       <c r="B25">
         <v>0.20071286399999999</v>
@@ -4557,13 +4585,14 @@
         <v>1.1883086110000001</v>
       </c>
       <c r="D25">
+        <f t="shared" si="1"/>
+        <v>0.14307166989383191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26">
         <f t="shared" si="0"/>
-        <v>0.6674337077905883</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
+        <v>11.999999986288</v>
       </c>
       <c r="B26">
         <v>0.20943951</v>
@@ -4572,13 +4601,14 @@
         <v>1.279691103</v>
       </c>
       <c r="D26">
+        <f t="shared" si="1"/>
+        <v>0.15209840908279482</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27">
         <f t="shared" si="0"/>
-        <v>0.7175404602483475</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
+        <v>12.499999971392722</v>
       </c>
       <c r="B27">
         <v>0.218166156</v>
@@ -4587,13 +4617,14 @@
         <v>1.3728757069999999</v>
       </c>
       <c r="D27">
+        <f t="shared" si="1"/>
+        <v>0.16139643154168759</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28">
         <f t="shared" si="0"/>
-        <v>0.76930035637750871</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
+        <v>13.000000013793224</v>
       </c>
       <c r="B28">
         <v>0.226892803</v>
@@ -4602,13 +4633,14 @@
         <v>1.4676990000000001</v>
       </c>
       <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.17096516483670765</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29">
         <f t="shared" si="0"/>
-        <v>0.82269107559213817</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
+        <v>13.499999998897946</v>
       </c>
       <c r="B29">
         <v>0.23561944900000001</v>
@@ -4617,13 +4649,14 @@
         <v>1.5640046889999999</v>
       </c>
       <c r="D29">
+        <f t="shared" si="1"/>
+        <v>0.18080401653036571</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30">
         <f t="shared" si="0"/>
-        <v>0.8776895753990499</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
+        <v>13.999999984002669</v>
       </c>
       <c r="B30">
         <v>0.24434609500000001</v>
@@ -4632,13 +4665,14 @@
         <v>1.6616436910000001</v>
       </c>
       <c r="D30">
+        <f t="shared" si="1"/>
+        <v>0.19091238079697614</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31">
         <f t="shared" si="0"/>
-        <v>0.93427213804469122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
+        <v>14.500000026403169</v>
       </c>
       <c r="B31">
         <v>0.25307274200000002</v>
@@ -4647,13 +4681,14 @@
         <v>1.7604741349999999</v>
       </c>
       <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0.20128963530958366</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32">
         <f t="shared" si="0"/>
-        <v>0.99241436321083842</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
+        <v>15.000000011507892</v>
       </c>
       <c r="B32">
         <v>0.26179938800000002</v>
@@ -4662,13 +4697,14 @@
         <v>1.860361274</v>
       </c>
       <c r="D32">
+        <f t="shared" si="1"/>
+        <v>0.21193513757200488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33">
         <f t="shared" si="0"/>
-        <v>1.0520911577381016</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
+        <v>15.499999996612614</v>
       </c>
       <c r="B33">
         <v>0.27052603400000003</v>
@@ -4677,13 +4713,14 @@
         <v>1.9611773480000001</v>
       </c>
       <c r="D33">
+        <f t="shared" si="1"/>
+        <v>0.22284823209330717</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34">
         <f t="shared" si="0"/>
-        <v>1.1132767864241471</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
+        <v>15.999999981717332</v>
       </c>
       <c r="B34">
         <v>0.27925267999999998</v>
@@ -4692,13 +4729,14 @@
         <v>2.0628013940000001</v>
       </c>
       <c r="D34">
+        <f t="shared" si="1"/>
+        <v>0.23402824570245517</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35">
         <f t="shared" si="0"/>
-        <v>1.1759448566524848</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>33</v>
+        <v>16.500000024117835</v>
       </c>
       <c r="B35">
         <v>0.28797932700000001</v>
@@ -4707,13 +4745,14 @@
         <v>2.1651190169999999</v>
       </c>
       <c r="D35">
+        <f t="shared" si="1"/>
+        <v>0.24547449009045863</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36">
         <f t="shared" si="0"/>
-        <v>1.2400683437810769</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
+        <v>17.000000009222557</v>
       </c>
       <c r="B36">
         <v>0.29670597300000001</v>
@@ -4722,13 +4761,14 @@
         <v>2.2680221459999999</v>
       </c>
       <c r="D36">
+        <f t="shared" si="1"/>
+        <v>0.25718625657581651</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37">
         <f t="shared" si="0"/>
-        <v>1.3056195732433147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
+        <v>17.499999994327279</v>
       </c>
       <c r="B37">
         <v>0.30543261900000002</v>
@@ -4737,13 +4777,14 @@
         <v>2.371408765</v>
       </c>
       <c r="D37">
+        <f t="shared" si="1"/>
+        <v>0.26916282401804992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38">
         <f t="shared" si="0"/>
-        <v>1.3725702765720036</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
+        <v>17.999999979432001</v>
       </c>
       <c r="B38">
         <v>0.31415926500000002</v>
@@ -4752,13 +4793,14 @@
         <v>2.475182631</v>
       </c>
       <c r="D38">
+        <f t="shared" si="1"/>
+        <v>0.2814034536461083</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39">
         <f t="shared" si="0"/>
-        <v>1.4408915743672814</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
+        <v>18.500000021832502</v>
       </c>
       <c r="B39">
         <v>0.322885912</v>
@@ -4767,13 +4809,14 @@
         <v>2.5792529989999999</v>
       </c>
       <c r="D39">
+        <f t="shared" si="1"/>
+        <v>0.29390739184824533</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40">
         <f t="shared" si="0"/>
-        <v>1.5105540040774068</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
+        <v>19.000000006937224</v>
       </c>
       <c r="B40">
         <v>0.331612558</v>
@@ -4782,13 +4825,14 @@
         <v>2.6835343360000001</v>
       </c>
       <c r="D40">
+        <f t="shared" si="1"/>
+        <v>0.30667386445702327</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41">
         <f t="shared" si="0"/>
-        <v>1.5815275006257985</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
+        <v>19.499999992041946</v>
       </c>
       <c r="B41">
         <v>0.34033920400000001</v>
@@ -4797,13 +4841,14 @@
         <v>2.7879460420000002</v>
       </c>
       <c r="D41">
+        <f t="shared" si="1"/>
+        <v>0.3197020853940975</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42">
         <f t="shared" si="0"/>
-        <v>1.6537814572743357</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
+        <v>19.999999977146668</v>
       </c>
       <c r="B42">
         <v>0.34906585000000001</v>
@@ -4812,13 +4857,14 @@
         <v>2.8924121810000001</v>
       </c>
       <c r="D42">
+        <f t="shared" si="1"/>
+        <v>0.33299125101747951</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43">
         <f t="shared" si="0"/>
-        <v>1.7272847070478865</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
+        <v>20.500000019547169</v>
       </c>
       <c r="B43">
         <v>0.35779249699999999</v>
@@ -4827,13 +4873,14 @@
         <v>2.9968612120000002</v>
       </c>
       <c r="D43">
+        <f t="shared" si="1"/>
+        <v>0.34654054315639193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44">
         <f t="shared" si="0"/>
-        <v>1.8020055527156509</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
+        <v>21.000000004651891</v>
       </c>
       <c r="B44">
         <v>0.36651914299999999</v>
@@ -4842,13 +4889,14 @@
         <v>3.1012257390000002</v>
       </c>
       <c r="D44">
+        <f t="shared" si="1"/>
+        <v>0.36034912292146881</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45">
         <f t="shared" si="0"/>
-        <v>1.877911746077896</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>43</v>
+        <v>21.499999989756613</v>
       </c>
       <c r="B45">
         <v>0.375245789</v>
@@ -4857,13 +4905,14 @@
         <v>3.2054422659999999</v>
       </c>
       <c r="D45">
+        <f t="shared" si="1"/>
+        <v>0.37441614007226498</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46">
         <f t="shared" si="0"/>
-        <v>1.954970553248736</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
+        <v>21.999999974861336</v>
       </c>
       <c r="B46">
         <v>0.383972435</v>
@@ -4872,13 +4921,14 @@
         <v>3.3094509639999998</v>
       </c>
       <c r="D46">
+        <f t="shared" si="1"/>
+        <v>0.38874072688895023</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47">
         <f t="shared" si="0"/>
-        <v>2.0331487346654105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>45</v>
+        <v>22.500000017261833</v>
       </c>
       <c r="B47">
         <v>0.39269908199999998</v>
@@ -4887,13 +4937,14 @@
         <v>3.4131954489999998</v>
       </c>
       <c r="D47">
+        <f t="shared" si="1"/>
+        <v>0.40332200144915209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48">
         <f t="shared" si="0"/>
-        <v>2.1124125770633682</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
+        <v>23.000000002366555</v>
       </c>
       <c r="B48">
         <v>0.40142572799999998</v>
@@ -4902,13 +4953,14 @@
         <v>3.5166225799999999</v>
       </c>
       <c r="D48">
+        <f t="shared" si="1"/>
+        <v>0.41815906096946254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49">
         <f t="shared" si="0"/>
-        <v>2.192727871565574</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>47</v>
+        <v>23.499999987471277</v>
       </c>
       <c r="B49">
         <v>0.41015237399999999</v>
@@ -4917,13 +4969,14 @@
         <v>3.6196822549999998</v>
       </c>
       <c r="D49">
+        <f t="shared" si="1"/>
+        <v>0.43325099188641492</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50">
         <f t="shared" si="0"/>
-        <v>2.2740599829344621</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>48</v>
+        <v>23.999999972575999</v>
       </c>
       <c r="B50">
         <v>0.41887901999999999</v>
@@ -4932,13 +4985,14 @@
         <v>3.7223272280000002</v>
       </c>
       <c r="D50">
+        <f t="shared" si="1"/>
+        <v>0.4485968632586772</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51">
         <f t="shared" si="0"/>
-        <v>2.3563738283038478</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>49</v>
+        <v>24.500000014976504</v>
       </c>
       <c r="B51">
         <v>0.42760566700000002</v>
@@ -4947,13 +5001,14 @@
         <v>3.8245129370000002</v>
       </c>
       <c r="D51">
+        <f t="shared" si="1"/>
+        <v>0.46419573028263006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52">
         <f t="shared" si="0"/>
-        <v>2.4396339109271956</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>50</v>
+        <v>25.000000000081226</v>
       </c>
       <c r="B52">
         <v>0.43633231300000003</v>
@@ -4962,13 +5017,14 @@
         <v>3.9261973389999998</v>
       </c>
       <c r="D52">
+        <f t="shared" si="1"/>
+        <v>0.48004662717175872</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53">
         <f t="shared" si="0"/>
-        <v>2.5238042972206398</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>51</v>
+        <v>25.499999985185944</v>
       </c>
       <c r="B53">
         <v>0.44505895899999998</v>
@@ -4977,13 +5033,14 @@
         <v>4.0273407580000002</v>
       </c>
       <c r="D53">
+        <f t="shared" si="1"/>
+        <v>0.49614857794115785</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54">
         <f t="shared" si="0"/>
-        <v>2.6088486895064058</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>52</v>
+        <v>26.000000027586449</v>
       </c>
       <c r="B54">
         <v>0.45378560600000001</v>
@@ -4992,13 +5049,14 @@
         <v>4.1279057410000002</v>
       </c>
       <c r="D54">
+        <f t="shared" si="1"/>
+        <v>0.51250059123480796</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55">
         <f t="shared" si="0"/>
-        <v>2.6947304135019525</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>53</v>
+        <v>26.500000012691171</v>
       </c>
       <c r="B55">
         <v>0.46251225200000001</v>
@@ -5007,13 +5065,14 @@
         <v>4.2278569250000002</v>
       </c>
       <c r="D55">
+        <f t="shared" si="1"/>
+        <v>0.52910165463597725</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56">
         <f t="shared" si="0"/>
-        <v>2.7814124041692181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>54</v>
+        <v>26.999999997795893</v>
       </c>
       <c r="B56">
         <v>0.47123889800000002</v>
@@ -5022,13 +5081,14 @@
         <v>4.3271609140000002</v>
       </c>
       <c r="D56">
+        <f t="shared" si="1"/>
+        <v>0.54595074597243354</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57">
         <f t="shared" si="0"/>
-        <v>2.8688572807485304</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>55</v>
+        <v>27.499999982900615</v>
       </c>
       <c r="B57">
         <v>0.47996554400000002</v>
@@ -5037,13 +5097,14 @@
         <v>4.4257861580000002</v>
       </c>
       <c r="D57">
+        <f t="shared" si="1"/>
+        <v>0.56304682591291844</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58">
         <f t="shared" si="0"/>
-        <v>2.9570273236128939</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>56</v>
+        <v>28.000000025301112</v>
       </c>
       <c r="B58">
         <v>0.488692191</v>
@@ -5052,13 +5113,14 @@
         <v>4.5237028500000003</v>
       </c>
       <c r="D58">
+        <f t="shared" si="1"/>
+        <v>0.58038884189205264</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59">
         <f t="shared" si="0"/>
-        <v>3.0458845105527117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>57</v>
+        <v>28.500000010405834</v>
       </c>
       <c r="B59">
         <v>0.497418837</v>
@@ -5067,13 +5129,14 @@
         <v>4.6208828219999996</v>
       </c>
       <c r="D59">
+        <f t="shared" si="1"/>
+        <v>0.59797572019819034</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60">
         <f t="shared" si="0"/>
-        <v>3.1353904923725677</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>58</v>
+        <v>28.999999995510553</v>
       </c>
       <c r="B60">
         <v>0.50614548299999995</v>
@@ -5082,13 +5145,14 @@
         <v>4.7172994490000004</v>
       </c>
       <c r="D60">
+        <f t="shared" si="1"/>
+        <v>0.61580637796307824</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61">
         <f t="shared" si="0"/>
-        <v>3.2255066705247724</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>59</v>
+        <v>29.499999980615279</v>
       </c>
       <c r="B61">
         <v>0.51487212900000001</v>
@@ -5097,13 +5161,14 @@
         <v>4.8129275639999998</v>
       </c>
       <c r="D61">
+        <f t="shared" si="1"/>
+        <v>0.63387971530782083</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62">
         <f t="shared" si="0"/>
-        <v>3.3161941731078635</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>60</v>
+        <v>30.000000023015783</v>
       </c>
       <c r="B62">
         <v>0.52359877600000004</v>
@@ -5112,13 +5177,14 @@
         <v>4.907743376</v>
       </c>
       <c r="D62">
+        <f t="shared" si="1"/>
+        <v>0.65219461949643476</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63">
         <f t="shared" si="0"/>
-        <v>3.407413892259755</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>61</v>
+        <v>30.500000008120502</v>
       </c>
       <c r="B63">
         <v>0.53232542199999999</v>
@@ -5127,13 +5193,14 @@
         <v>5.0017243899999997</v>
       </c>
       <c r="D63">
+        <f t="shared" si="1"/>
+        <v>0.67074995658198189</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64">
         <f t="shared" si="0"/>
-        <v>3.4991264591577753</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>62</v>
+        <v>30.999999993225227</v>
       </c>
       <c r="B64">
         <v>0.54105206800000005</v>
@@ -5142,13 +5209,14 @@
         <v>5.0948493399999997</v>
       </c>
       <c r="D64">
+        <f t="shared" si="1"/>
+        <v>0.689544584068849</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65">
         <f t="shared" si="0"/>
-        <v>3.5912923237163374</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>63</v>
+        <v>31.499999978329946</v>
       </c>
       <c r="B65">
         <v>0.549778714</v>
@@ -5157,13 +5225,14 @@
         <v>5.187098121</v>
       </c>
       <c r="D65">
+        <f t="shared" si="1"/>
+        <v>0.70857734261595162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66">
         <f t="shared" si="0"/>
-        <v>3.68387172989519</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>64</v>
+        <v>32.000000020730447</v>
       </c>
       <c r="B66">
         <v>0.55850536100000003</v>
@@ -5172,13 +5241,14 @@
         <v>5.2784517260000001</v>
       </c>
       <c r="D66">
-        <f t="shared" si="0"/>
-        <v>3.7768247539430955</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.72784706041483771</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67">
-        <v>65</v>
+        <f t="shared" ref="A67:A130" si="2">DEGREES(B67)</f>
+        <v>32.500000005835169</v>
       </c>
       <c r="B67">
         <v>0.56723200699999998</v>
@@ -5187,13 +5257,14 @@
         <v>5.3688921890000003</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D130" si="1">$H$2*SIN($H$3*B67 + $H$5)+$H$4</f>
-        <v>3.8701112789735439</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D67:D130" si="3">$H$2*SIN($H$3*B67 + $H$5)+$H$4</f>
+        <v>0.74735254440234478</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>66</v>
+        <f t="shared" si="2"/>
+        <v>32.999999990939891</v>
       </c>
       <c r="B68">
         <v>0.57595865300000004</v>
@@ -5202,13 +5273,14 @@
         <v>5.4584025340000002</v>
       </c>
       <c r="D68">
-        <f t="shared" si="1"/>
-        <v>3.9636910761768016</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.76709259358300752</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>67</v>
+        <f t="shared" si="2"/>
+        <v>33.499999976044613</v>
       </c>
       <c r="B69">
         <v>0.58468529899999999</v>
@@ -5217,13 +5289,14 @@
         <v>5.5469667190000003</v>
       </c>
       <c r="D69">
-        <f t="shared" si="1"/>
-        <v>4.0575237796082515</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.7870659902976791</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>68</v>
+        <f t="shared" si="2"/>
+        <v>34.000000018445114</v>
       </c>
       <c r="B70">
         <v>0.59341194600000002</v>
@@ -5232,13 +5305,14 @@
         <v>5.6345695940000002</v>
       </c>
       <c r="D70">
-        <f t="shared" si="1"/>
-        <v>4.1515689250187746</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.8072715048218746</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>69</v>
+        <f t="shared" si="2"/>
+        <v>34.500000003549836</v>
       </c>
       <c r="B71">
         <v>0.60213859199999997</v>
@@ -5247,13 +5321,14 @@
         <v>5.7211968549999996</v>
       </c>
       <c r="D71">
-        <f t="shared" si="1"/>
-        <v>4.2457859241815354</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.82770788615361646</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72">
-        <v>70</v>
+        <f t="shared" si="2"/>
+        <v>34.999999988654558</v>
       </c>
       <c r="B72">
         <v>0.61086523800000003</v>
@@ -5262,13 +5337,14 @@
         <v>5.8068350009999996</v>
       </c>
       <c r="D72">
-        <f t="shared" si="1"/>
-        <v>4.3401341470582002</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.84837387598282232</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73">
-        <v>71</v>
+        <f t="shared" si="2"/>
+        <v>35.49999997375928</v>
       </c>
       <c r="B73">
         <v>0.61959188399999998</v>
@@ -5277,13 +5353,14 @@
         <v>5.8914713030000003</v>
       </c>
       <c r="D73">
-        <f t="shared" si="1"/>
-        <v>4.4345728962412823</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.86926819953396794</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74">
-        <v>72</v>
+        <f t="shared" si="2"/>
+        <v>36.000000016159781</v>
       </c>
       <c r="B74">
         <v>0.62831853100000001</v>
@@ -5292,13 +5369,14 @@
         <v>5.9750937579999999</v>
       </c>
       <c r="D74">
-        <f t="shared" si="1"/>
-        <v>4.5290614461033742</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.89038957038012434</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75">
-        <v>73</v>
+        <f t="shared" si="2"/>
+        <v>36.500000001264503</v>
       </c>
       <c r="B75">
         <v>0.63704517699999996</v>
@@ -5307,13 +5385,14 @@
         <v>6.0576910650000002</v>
       </c>
       <c r="D75">
-        <f t="shared" si="1"/>
-        <v>4.6235590170520959</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.91173668081508685</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76">
-        <v>74</v>
+        <f t="shared" si="2"/>
+        <v>36.999999986369225</v>
       </c>
       <c r="B76">
         <v>0.64577182300000002</v>
@@ -5322,13 +5401,14 @@
         <v>6.1392525859999996</v>
       </c>
       <c r="D76">
-        <f t="shared" si="1"/>
-        <v>4.7180248580837105</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.93330821645595607</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77">
-        <v>75</v>
+        <f t="shared" si="2"/>
+        <v>37.499999971473947</v>
       </c>
       <c r="B77">
         <v>0.65449846899999997</v>
@@ -5337,13 +5417,14 @@
         <v>6.21976832</v>
       </c>
       <c r="D77">
-        <f t="shared" si="1"/>
-        <v>4.8124182210557649</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.95510284666888134</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78">
-        <v>76</v>
+        <f t="shared" si="2"/>
+        <v>38.000000013874448</v>
       </c>
       <c r="B78">
         <v>0.663225116</v>
@@ -5352,13 +5433,14 @@
         <v>6.2992288780000001</v>
       </c>
       <c r="D78">
-        <f t="shared" si="1"/>
-        <v>4.9066983998851255</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.97711922959403452</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79">
-        <v>77</v>
+        <f t="shared" si="2"/>
+        <v>38.499999998979163</v>
       </c>
       <c r="B79">
         <v>0.67195176199999995</v>
@@ -5367,13 +5449,14 @@
         <v>6.3776254520000002</v>
       </c>
       <c r="D79">
-        <f t="shared" si="1"/>
-        <v>5.0008247049086751</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>0.99935600211153419</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80">
-        <v>78</v>
+        <f t="shared" si="2"/>
+        <v>38.999999984083892</v>
       </c>
       <c r="B80">
         <v>0.68067840800000001</v>
@@ -5382,13 +5465,14 @@
         <v>6.454949794</v>
       </c>
       <c r="D80">
-        <f t="shared" si="1"/>
-        <v>5.0947565452548824</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.021811795062801</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81">
-        <v>79</v>
+        <f t="shared" si="2"/>
+        <v>39.500000026484393</v>
       </c>
       <c r="B81">
         <v>0.68940505500000004</v>
@@ -5397,13 +5481,14 @@
         <v>6.5311941899999999</v>
       </c>
       <c r="D81">
-        <f t="shared" si="1"/>
-        <v>5.1884534138460578</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.0444852258794319</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82">
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>40.000000011589115</v>
       </c>
       <c r="B82">
         <v>0.69813170099999999</v>
@@ -5412,13 +5497,14 @@
         <v>6.6063514420000002</v>
       </c>
       <c r="D82">
-        <f t="shared" si="1"/>
-        <v>5.2818748727655009</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.0673748907611547</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83">
-        <v>81</v>
+        <f t="shared" si="2"/>
+        <v>40.499999996693838</v>
       </c>
       <c r="B83">
         <v>0.70685834700000005</v>
@@ -5427,13 +5513,14 @@
         <v>6.6804148489999999</v>
       </c>
       <c r="D83">
-        <f t="shared" si="1"/>
-        <v>5.3749806351194316</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.0904793803514456</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84">
-        <v>82</v>
+        <f t="shared" si="2"/>
+        <v>40.99999998179856</v>
       </c>
       <c r="B84">
         <v>0.715584993</v>
@@ -5442,13 +5529,14 @@
         <v>6.7533781810000004</v>
       </c>
       <c r="D84">
-        <f t="shared" si="1"/>
-        <v>5.46773053943968</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.1137972694566387</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85">
-        <v>83</v>
+        <f t="shared" si="2"/>
+        <v>41.500000024199061</v>
       </c>
       <c r="B85">
         <v>0.72431164000000003</v>
@@ -5457,13 +5545,14 @@
         <v>6.8252356670000003</v>
       </c>
       <c r="D85">
-        <f t="shared" si="1"/>
-        <v>5.5600845883173715</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.1373271224279948</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86">
-        <v>84</v>
+        <f t="shared" si="2"/>
+        <v>42.000000009303783</v>
       </c>
       <c r="B86">
         <v>0.73303828599999998</v>
@@ -5472,13 +5561,14 @@
         <v>6.8959819790000001</v>
       </c>
       <c r="D86">
-        <f t="shared" si="1"/>
-        <v>5.6520029233731197</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.1610674824408158</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87">
-        <v>85</v>
+        <f t="shared" si="2"/>
+        <v>42.499999994408505</v>
       </c>
       <c r="B87">
         <v>0.74176493200000004</v>
@@ -5487,13 +5577,14 @@
         <v>6.9656122089999997</v>
       </c>
       <c r="D87">
-        <f t="shared" si="1"/>
-        <v>5.7434459059457597</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.1850168877621621</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88">
-        <v>86</v>
+        <f t="shared" si="2"/>
+        <v>42.999999979513227</v>
       </c>
       <c r="B88">
         <v>0.75049157799999999</v>
@@ -5502,13 +5593,14 @@
         <v>7.0341218620000001</v>
       </c>
       <c r="D88">
-        <f t="shared" si="1"/>
-        <v>5.834374091812494</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.2091738610799903</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89">
-        <v>87</v>
+        <f t="shared" si="2"/>
+        <v>43.500000021913728</v>
       </c>
       <c r="B89">
         <v>0.75921822500000002</v>
@@ -5517,13 +5609,14 @@
         <v>7.1015068369999996</v>
       </c>
       <c r="D89">
-        <f t="shared" si="1"/>
-        <v>5.9247482691326177</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.2335369150820346</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90">
-        <v>88</v>
+        <f t="shared" si="2"/>
+        <v>44.000000007018443</v>
       </c>
       <c r="B90">
         <v>0.76794487099999997</v>
@@ -5532,13 +5625,14 @@
         <v>7.1677634140000004</v>
       </c>
       <c r="D90">
-        <f t="shared" si="1"/>
-        <v>6.014529434004408</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.2581045413568828</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91">
-        <v>89</v>
+        <f t="shared" si="2"/>
+        <v>44.499999992123172</v>
       </c>
       <c r="B91">
         <v>0.77667151700000003</v>
@@ -5547,13 +5641,14 @@
         <v>7.2328882429999997</v>
       </c>
       <c r="D91">
-        <f t="shared" si="1"/>
-        <v>6.1036788694240576</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.2828752272377346</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92">
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>44.999999977227887</v>
       </c>
       <c r="B92">
         <v>0.78539816299999998</v>
@@ -5562,13 +5657,14 @@
         <v>7.2968783310000003</v>
       </c>
       <c r="D92">
-        <f t="shared" si="1"/>
-        <v>6.1921581204976643</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.3078474447520936</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93">
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>45.500000019628395</v>
       </c>
       <c r="B93">
         <v>0.79412481000000001</v>
@@ -5577,13 +5673,14 @@
         <v>7.3597310279999997</v>
       </c>
       <c r="D93">
-        <f t="shared" si="1"/>
-        <v>6.2799290314332605</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.333019656391969</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94">
-        <v>92</v>
+        <f t="shared" si="2"/>
+        <v>46.00000000473311</v>
       </c>
       <c r="B94">
         <v>0.80285145599999996</v>
@@ -5592,13 +5689,14 @@
         <v>7.42144402</v>
       </c>
       <c r="D94">
-        <f t="shared" si="1"/>
-        <v>6.366953721853001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.3583903036478522</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95">
-        <v>93</v>
+        <f t="shared" si="2"/>
+        <v>46.499999989837839</v>
       </c>
       <c r="B95">
         <v>0.81157810200000002</v>
@@ -5607,13 +5705,14 @@
         <v>7.4820153180000002</v>
       </c>
       <c r="D95">
-        <f t="shared" si="1"/>
-        <v>6.4531946634776531</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.3839578244119006</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96">
-        <v>94</v>
+        <f t="shared" si="2"/>
+        <v>46.999999974942554</v>
       </c>
       <c r="B96">
         <v>0.82030474799999997</v>
@@ -5622,13 +5721,14 @@
         <v>7.5414432439999999</v>
       </c>
       <c r="D96">
-        <f t="shared" si="1"/>
-        <v>6.5386146560014096</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.4097206415590935</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97">
-        <v>95</v>
+        <f t="shared" si="2"/>
+        <v>47.500000017343062</v>
       </c>
       <c r="B97">
         <v>0.829031395</v>
@@ -5637,13 +5737,14 @@
         <v>7.5997264270000002</v>
       </c>
       <c r="D97">
-        <f t="shared" si="1"/>
-        <v>6.6231768628770542</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.4356771689030463</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98">
-        <v>96</v>
+        <f t="shared" si="2"/>
+        <v>48.000000002447777</v>
       </c>
       <c r="B98">
         <v>0.83775804099999995</v>
@@ -5652,13 +5753,14 @@
         <v>7.6568637920000002</v>
       </c>
       <c r="D98">
-        <f t="shared" si="1"/>
-        <v>6.7068447885468503</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.461825799374215</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99">
-        <v>97</v>
+        <f t="shared" si="2"/>
+        <v>48.499999987552506</v>
       </c>
       <c r="B99">
         <v>0.84648468700000001</v>
@@ -5667,13 +5769,14 @@
         <v>7.7128545480000001</v>
       </c>
       <c r="D99">
-        <f t="shared" si="1"/>
-        <v>6.7895823523236132</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.4881649229653284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100">
-        <v>98</v>
+        <f t="shared" si="2"/>
+        <v>48.999999972657221</v>
       </c>
       <c r="B100">
         <v>0.85521133299999996</v>
@@ -5682,13 +5785,14 @@
         <v>7.7676981850000004</v>
       </c>
       <c r="D100">
-        <f t="shared" si="1"/>
-        <v>6.8713538650947665</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.5146929149552708</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101">
-        <v>99</v>
+        <f t="shared" si="2"/>
+        <v>49.500000015057722</v>
       </c>
       <c r="B101">
         <v>0.86393797999999999</v>
@@ -5697,13 +5801,14 @@
         <v>7.821394465</v>
       </c>
       <c r="D101">
-        <f t="shared" si="1"/>
-        <v>6.9521240636538018</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.5414081420446406</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102">
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>50.000000000162451</v>
       </c>
       <c r="B102">
         <v>0.87266462600000005</v>
@@ -5712,13 +5817,14 @@
         <v>7.8739434109999999</v>
       </c>
       <c r="D102">
-        <f t="shared" si="1"/>
-        <v>7.0318580890069278</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.568308950189842</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103">
-        <v>101</v>
+        <f t="shared" si="2"/>
+        <v>50.499999985267166</v>
       </c>
       <c r="B103">
         <v>0.881391272</v>
@@ -5727,13 +5833,14 @@
         <v>7.9253453040000004</v>
       </c>
       <c r="D103">
-        <f t="shared" si="1"/>
-        <v>7.1105215569410882</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.5953936830730564</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104">
-        <v>102</v>
+        <f t="shared" si="2"/>
+        <v>51.000000027667674</v>
       </c>
       <c r="B104">
         <v>0.89011791900000004</v>
@@ -5742,13 +5849,14 @@
         <v>7.9756006729999998</v>
       </c>
       <c r="D104">
-        <f t="shared" si="1"/>
-        <v>7.1880805445410143</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.6226606731154223</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105">
-        <v>103</v>
+        <f t="shared" si="2"/>
+        <v>51.500000012772389</v>
       </c>
       <c r="B105">
         <v>0.89884456499999998</v>
@@ -5757,13 +5865,14 @@
         <v>8.0247102909999999</v>
       </c>
       <c r="D105">
-        <f t="shared" si="1"/>
-        <v>7.2645015787149454</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.6501082321115557</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106">
-        <v>104</v>
+        <f t="shared" si="2"/>
+        <v>51.999999997877119</v>
       </c>
       <c r="B106">
         <v>0.90757121100000004</v>
@@ -5772,13 +5881,14 @@
         <v>8.0726751659999998</v>
       </c>
       <c r="D106">
-        <f t="shared" si="1"/>
-        <v>7.339751703957079</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.6777346700809845</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107">
-        <v>105</v>
+        <f t="shared" si="2"/>
+        <v>52.499999982981834</v>
       </c>
       <c r="B107">
         <v>0.91629785699999999</v>
@@ -5787,13 +5897,14 @@
         <v>8.1194965369999998</v>
       </c>
       <c r="D107">
-        <f t="shared" si="1"/>
-        <v>7.4137984608853786</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.7055382828949837</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108">
-        <v>106</v>
+        <f t="shared" si="2"/>
+        <v>53.000000025382342</v>
       </c>
       <c r="B108">
         <v>0.92502450400000003</v>
@@ -5802,13 +5913,14 @@
         <v>8.1651758680000004</v>
       </c>
       <c r="D108">
-        <f t="shared" si="1"/>
-        <v>7.48660991746618</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.7335173587120041</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109">
-        <v>107</v>
+        <f t="shared" si="2"/>
+        <v>53.500000010487057</v>
       </c>
       <c r="B109">
         <v>0.93375114999999997</v>
@@ -5817,13 +5929,14 @@
         <v>8.2097148410000003</v>
       </c>
       <c r="D109">
-        <f t="shared" si="1"/>
-        <v>7.5581546495584142</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.7616701652386606</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110">
-        <v>108</v>
+        <f t="shared" si="2"/>
+        <v>53.999999995591786</v>
       </c>
       <c r="B110">
         <v>0.94247779600000003</v>
@@ -5832,13 +5945,14 @@
         <v>8.2531153479999997</v>
       </c>
       <c r="D110">
-        <f t="shared" si="1"/>
-        <v>7.6284018045281972</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.7899949690734838</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111">
-        <v>109</v>
+        <f t="shared" si="2"/>
+        <v>54.499999980696501</v>
       </c>
       <c r="B111">
         <v>0.95120444199999998</v>
@@ -5847,13 +5961,14 @@
         <v>8.2953794940000005</v>
       </c>
       <c r="D111">
-        <f t="shared" si="1"/>
-        <v>7.6973210810407107</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.8184900230092547</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112">
-        <v>110</v>
+        <f t="shared" si="2"/>
+        <v>55.000000023097002</v>
       </c>
       <c r="B112">
         <v>0.95993108900000002</v>
@@ -5862,13 +5977,14 @@
         <v>8.3365095819999997</v>
       </c>
       <c r="D112">
-        <f t="shared" si="1"/>
-        <v>7.7648827582088522</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.8471535726311155</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113">
-        <v>111</v>
+        <f t="shared" si="2"/>
+        <v>55.500000008201724</v>
       </c>
       <c r="B113">
         <v>0.96865773499999996</v>
@@ -5877,13 +5993,14 @@
         <v>8.376508115</v>
       </c>
       <c r="D113">
-        <f t="shared" si="1"/>
-        <v>7.8310576776038019</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.8759838432672455</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114">
-        <v>112</v>
+        <f t="shared" si="2"/>
+        <v>55.999999993306446</v>
       </c>
       <c r="B114">
         <v>0.97738438100000002</v>
@@ -5892,13 +6009,14 @@
         <v>8.4153777880000007</v>
       </c>
       <c r="D114">
-        <f t="shared" si="1"/>
-        <v>7.895817302282925</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.9049790598058371</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115">
-        <v>113</v>
+        <f t="shared" si="2"/>
+        <v>56.499999978411168</v>
       </c>
       <c r="B115">
         <v>0.98611102699999997</v>
@@ -5907,13 +6025,14 @@
         <v>8.4531214820000002</v>
       </c>
       <c r="D115">
-        <f t="shared" si="1"/>
-        <v>7.959133697975135</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.9341374336854593</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116">
-        <v>114</v>
+        <f t="shared" si="2"/>
+        <v>57.000000020811669</v>
       </c>
       <c r="B116">
         <v>0.99483767400000001</v>
@@ -5922,13 +6041,14 @@
         <v>8.4897422640000002</v>
       </c>
       <c r="D116">
-        <f t="shared" si="1"/>
-        <v>8.0209795599525187</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.9634571696493408</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117">
-        <v>115</v>
+        <f t="shared" si="2"/>
+        <v>57.500000005916391</v>
       </c>
       <c r="B117">
         <v>1.00356432</v>
@@ -5937,13 +6057,14 @@
         <v>8.5252433790000008</v>
       </c>
       <c r="D117">
-        <f t="shared" si="1"/>
-        <v>8.0813281966313291</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>1.9929364523986131</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118">
-        <v>116</v>
+        <f t="shared" si="2"/>
+        <v>57.999999991021106</v>
       </c>
       <c r="B118">
         <v>1.0122909659999999</v>
@@ -5952,13 +6073,14 @@
         <v>8.5596282450000007</v>
       </c>
       <c r="D118">
-        <f t="shared" si="1"/>
-        <v>8.1401535836060344</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.0225734668629491</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119">
-        <v>117</v>
+        <f t="shared" si="2"/>
+        <v>58.499999976125842</v>
       </c>
       <c r="B119">
         <v>1.0210176120000001</v>
@@ -5967,13 +6089,14 @@
         <v>8.5929004510000002</v>
       </c>
       <c r="D119">
-        <f t="shared" si="1"/>
-        <v>8.1974303463579599</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.0523663848918021</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120">
-        <v>118</v>
+        <f t="shared" si="2"/>
+        <v>59.000000018526343</v>
       </c>
       <c r="B120">
         <v>1.0297442590000001</v>
@@ -5982,13 +6105,14 @@
         <v>8.6250637539999992</v>
       </c>
       <c r="D120">
-        <f t="shared" si="1"/>
-        <v>8.253133784664497</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.0823133721581892</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121">
-        <v>119</v>
+        <f t="shared" si="2"/>
+        <v>59.500000003631065</v>
       </c>
       <c r="B121">
         <v>1.0384709050000001</v>
@@ -5997,13 +6121,14 @@
         <v>8.6561220690000003</v>
       </c>
       <c r="D121">
-        <f t="shared" si="1"/>
-        <v>8.3072398579036744</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.1124125745276738</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A122">
-        <v>120</v>
+        <f t="shared" si="2"/>
+        <v>59.99999998873578</v>
       </c>
       <c r="B122">
         <v>1.047197551</v>
@@ -6012,13 +6137,14 @@
         <v>8.6860794729999995</v>
       </c>
       <c r="D122">
-        <f t="shared" si="1"/>
-        <v>8.3597252337216226</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.1426621387626645</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A123">
-        <v>121</v>
+        <f t="shared" si="2"/>
+        <v>60.499999973840502</v>
       </c>
       <c r="B123">
         <v>1.055924197</v>
@@ -6027,13 +6153,14 @@
         <v>8.7149401950000005</v>
       </c>
       <c r="D123">
-        <f t="shared" si="1"/>
-        <v>8.4105672723837372</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.1730601989276632</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A124">
-        <v>122</v>
+        <f t="shared" si="2"/>
+        <v>61.000000016241003</v>
       </c>
       <c r="B124">
         <v>1.064650844</v>
@@ -6042,13 +6169,14 @@
         <v>8.7427086149999997</v>
       </c>
       <c r="D124">
-        <f t="shared" si="1"/>
-        <v>8.459744048553155</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.2036048834357342</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A125">
-        <v>123</v>
+        <f t="shared" si="2"/>
+        <v>61.500000001345725</v>
       </c>
       <c r="B125">
         <v>1.0733774899999999</v>
@@ -6057,13 +6185,14 @@
         <v>8.7693892590000004</v>
       </c>
       <c r="D125">
-        <f t="shared" si="1"/>
-        <v>8.507234338400222</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.2342943011466811</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126">
-        <v>124</v>
+        <f t="shared" si="2"/>
+        <v>61.999999986450455</v>
       </c>
       <c r="B126">
         <v>1.0821041360000001</v>
@@ -6072,13 +6201,14 @@
         <v>8.794986797</v>
       </c>
       <c r="D126">
-        <f t="shared" si="1"/>
-        <v>8.5530176625676972</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.2651265624845713</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127">
-        <v>125</v>
+        <f t="shared" si="2"/>
+        <v>62.49999997155517</v>
       </c>
       <c r="B127">
         <v>1.0908307820000001</v>
@@ -6087,13 +6217,14 @@
         <v>8.8195060380000001</v>
       </c>
       <c r="D127">
-        <f t="shared" si="1"/>
-        <v>8.5970742722723728</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.2960997655704034</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128">
-        <v>126</v>
+        <f t="shared" si="2"/>
+        <v>63.000000013955678</v>
       </c>
       <c r="B128">
         <v>1.0995574290000001</v>
@@ -6102,13 +6233,14 @@
         <v>8.8429519259999996</v>
       </c>
       <c r="D128">
-        <f t="shared" si="1"/>
-        <v>8.6393851683025868</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.3272120034043224</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129">
-        <v>127</v>
+        <f t="shared" si="2"/>
+        <v>63.499999999060392</v>
       </c>
       <c r="B129">
         <v>1.108284075</v>
@@ -6117,13 +6249,14 @@
         <v>8.8653295389999993</v>
       </c>
       <c r="D129">
-        <f t="shared" si="1"/>
-        <v>8.6799320900215129</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.358461349706698</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A130">
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>63.999999984165115</v>
       </c>
       <c r="B130">
         <v>1.117010721</v>
@@ -6132,13 +6265,14 @@
         <v>8.8866440840000003</v>
       </c>
       <c r="D130">
-        <f t="shared" si="1"/>
-        <v>8.718697552333726</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>2.3898458804280378</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131">
-        <v>129</v>
+        <f t="shared" ref="A131:A182" si="4">DEGREES(B131)</f>
+        <v>64.500000026565615</v>
       </c>
       <c r="B131">
         <v>1.125737368</v>
@@ -6147,13 +6281,14 @@
         <v>8.9069008929999995</v>
       </c>
       <c r="D131">
-        <f t="shared" ref="D131:D182" si="2">$H$2*SIN($H$3*B131 + $H$5)+$H$4</f>
-        <v>8.7556648377656501</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D131:D182" si="5">$H$2*SIN($H$3*B131 + $H$5)+$H$4</f>
+        <v>2.4213636632420013</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A132">
-        <v>130</v>
+        <f t="shared" si="4"/>
+        <v>65.000000011670338</v>
       </c>
       <c r="B132">
         <v>1.134464014</v>
@@ -6162,13 +6297,14 @@
         <v>8.9261054200000007</v>
       </c>
       <c r="D132">
-        <f t="shared" si="2"/>
-        <v>8.7908179918885949</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.4530127467600895</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A133">
-        <v>131</v>
+        <f t="shared" si="4"/>
+        <v>65.49999999677506</v>
       </c>
       <c r="B133">
         <v>1.1431906599999999</v>
@@ -6177,13 +6313,14 @@
         <v>8.9442632389999996</v>
       </c>
       <c r="D133">
-        <f t="shared" si="2"/>
-        <v>8.8241418556166522</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.4847911823219433</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A134">
-        <v>132</v>
+        <f t="shared" si="4"/>
+        <v>65.999999981879782</v>
       </c>
       <c r="B134">
         <v>1.1519173060000001</v>
@@ -6192,13 +6329,14 @@
         <v>8.9613800399999999</v>
       </c>
       <c r="D134">
-        <f t="shared" si="2"/>
-        <v>8.8556220545946989</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.5166970096840848</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A135">
-        <v>133</v>
+        <f t="shared" si="4"/>
+        <v>66.500000024280283</v>
       </c>
       <c r="B135">
         <v>1.1606439529999999</v>
@@ -6207,13 +6345,14 @@
         <v>8.9774616260000002</v>
       </c>
       <c r="D135">
-        <f t="shared" si="2"/>
-        <v>8.8852450130259193</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.548728264422528</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A136">
-        <v>134</v>
+        <f t="shared" si="4"/>
+        <v>67.000000009385005</v>
       </c>
       <c r="B136">
         <v>1.1693705990000001</v>
@@ -6222,13 +6361,14 @@
         <v>8.9925139099999996</v>
       </c>
       <c r="D136">
-        <f t="shared" si="2"/>
-        <v>8.912997946163685</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.5808829633577379</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A137">
-        <v>135</v>
+        <f t="shared" si="4"/>
+        <v>67.499999994489727</v>
       </c>
       <c r="B137">
         <v>1.178097245</v>
@@ -6237,13 +6377,14 @@
         <v>9.0065429090000002</v>
       </c>
       <c r="D137">
-        <f t="shared" si="2"/>
-        <v>8.9388688861927879</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.6131591266998981</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A138">
-        <v>136</v>
+        <f t="shared" si="4"/>
+        <v>67.999999979594449</v>
       </c>
       <c r="B138">
         <v>1.186823891</v>
@@ -6252,13 +6393,14 @@
         <v>9.0195547479999991</v>
       </c>
       <c r="D138">
-        <f t="shared" si="2"/>
-        <v>8.9628466736005592</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.6455547635033416</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139">
-        <v>137</v>
+        <f t="shared" si="4"/>
+        <v>68.50000002199495</v>
       </c>
       <c r="B139">
         <v>1.195550538</v>
@@ -6267,13 +6409,14 @@
         <v>9.0315556499999996</v>
       </c>
       <c r="D139">
-        <f t="shared" si="2"/>
-        <v>8.9849209679118616</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.678067879185094</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140">
-        <v>138</v>
+        <f t="shared" si="4"/>
+        <v>69.000000007099672</v>
       </c>
       <c r="B140">
         <v>1.2042771839999999</v>
@@ -6282,13 +6425,14 @@
         <v>9.0425519360000006</v>
       </c>
       <c r="D140">
-        <f t="shared" si="2"/>
-        <v>9.0050822422504151</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.7106964607317288</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141">
-        <v>139</v>
+        <f t="shared" si="4"/>
+        <v>69.49999999220438</v>
       </c>
       <c r="B141">
         <v>1.2130038299999999</v>
@@ -6297,13 +6441,14 @@
         <v>9.0525500220000001</v>
       </c>
       <c r="D141">
-        <f t="shared" si="2"/>
-        <v>9.0233218026248778</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.7434384991777998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A142">
-        <v>140</v>
+        <f t="shared" si="4"/>
+        <v>69.999999977309116</v>
       </c>
       <c r="B142">
         <v>1.2217304760000001</v>
@@ -6312,13 +6457,14 @@
         <v>9.0615564160000002</v>
       </c>
       <c r="D142">
-        <f t="shared" si="2"/>
-        <v>9.0396317813425888</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.7762919748402668</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143">
-        <v>141</v>
+        <f t="shared" si="4"/>
+        <v>70.500000019709617</v>
       </c>
       <c r="B143">
         <v>1.2304571230000001</v>
@@ -6327,13 +6473,14 @@
         <v>9.0695777149999994</v>
       </c>
       <c r="D143">
-        <f t="shared" si="2"/>
-        <v>9.0540051445779568</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.8092548649455775</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144">
-        <v>142</v>
+        <f t="shared" si="4"/>
+        <v>71.000000004814339</v>
       </c>
       <c r="B144">
         <v>1.239183769</v>
@@ -6342,13 +6489,14 @@
         <v>9.0766206020000002</v>
       </c>
       <c r="D144">
-        <f t="shared" si="2"/>
-        <v>9.0664356890408015</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.8423251286330231</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A145">
-        <v>143</v>
+        <f t="shared" si="4"/>
+        <v>71.499999989919061</v>
       </c>
       <c r="B145">
         <v>1.247910415</v>
@@ -6357,13 +6505,14 @@
         <v>9.0826918449999994</v>
       </c>
       <c r="D145">
-        <f t="shared" si="2"/>
-        <v>9.0769180545341897</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.8755007297441257</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146">
-        <v>144</v>
+        <f t="shared" si="4"/>
+        <v>71.999999975023783</v>
       </c>
       <c r="B146">
         <v>1.2566370609999999</v>
@@ -6372,13 +6521,14 @@
         <v>9.0877982910000004</v>
       </c>
       <c r="D146">
-        <f t="shared" si="2"/>
-        <v>9.0854477194562655</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.9087796218516599</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A147">
-        <v>145</v>
+        <f t="shared" si="4"/>
+        <v>72.500000017424284</v>
       </c>
       <c r="B147">
         <v>1.265363708</v>
@@ -6387,13 +6537,14 @@
         <v>9.0919468650000006</v>
       </c>
       <c r="D147">
-        <f t="shared" si="2"/>
-        <v>9.0920210051498351</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.9421597559877268</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A148">
-        <v>146</v>
+        <f t="shared" si="4"/>
+        <v>73.000000002529006</v>
       </c>
       <c r="B148">
         <v>1.2740903539999999</v>
@@ -6402,13 +6553,14 @@
         <v>9.0951445690000003</v>
       </c>
       <c r="D148">
-        <f t="shared" si="2"/>
-        <v>9.096635074700675</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.9756390654584197</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A149">
-        <v>147</v>
+        <f t="shared" si="4"/>
+        <v>73.499999987633728</v>
       </c>
       <c r="B149">
         <v>1.2828170000000001</v>
@@ -6417,13 +6569,14 @@
         <v>9.0973984750000003</v>
       </c>
       <c r="D149">
-        <f t="shared" si="2"/>
-        <v>9.0992879386805345</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.0092154889216713</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A150">
-        <v>148</v>
+        <f t="shared" si="4"/>
+        <v>73.999999972738451</v>
       </c>
       <c r="B150">
         <v>1.291543646</v>
@@ -6432,13 +6585,14 @@
         <v>9.0987157270000001</v>
       </c>
       <c r="D150">
-        <f t="shared" si="2"/>
-        <v>9.0999784527680561</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.0428869552256463</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A151">
-        <v>149</v>
+        <f t="shared" si="4"/>
+        <v>74.500000015138951</v>
       </c>
       <c r="B151">
         <v>1.3002702930000001</v>
@@ -6447,17 +6601,14 @@
         <v>9.0991035369999995</v>
       </c>
       <c r="D151">
-        <f t="shared" si="2"/>
-        <v>9.0987063188495689</v>
-      </c>
-      <c r="E151">
-        <f>DEGREES(B151)</f>
-        <v>74.500000015138951</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.0766513912301869</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A152">
-        <v>150</v>
+        <f t="shared" si="4"/>
+        <v>75.000000000243674</v>
       </c>
       <c r="B152">
         <v>1.308996939</v>
@@ -6466,13 +6617,14 @@
         <v>9.0985691800000001</v>
       </c>
       <c r="D152">
-        <f t="shared" si="2"/>
-        <v>9.0954720859556453</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.1105067064477594</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A153">
-        <v>151</v>
+        <f t="shared" si="4"/>
+        <v>75.499999985348396</v>
       </c>
       <c r="B153">
         <v>1.317723585</v>
@@ -6481,13 +6633,14 @@
         <v>9.0971199949999999</v>
       </c>
       <c r="D153">
-        <f t="shared" si="2"/>
-        <v>9.090277149149653</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.1444508163870077</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A154">
-        <v>152</v>
+        <f t="shared" si="4"/>
+        <v>76.000000027748897</v>
       </c>
       <c r="B154">
         <v>1.326450232</v>
@@ -6496,13 +6649,14 @@
         <v>9.0947633779999997</v>
       </c>
       <c r="D154">
-        <f t="shared" si="2"/>
-        <v>9.0831237483523672</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.1784816311199942</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A155">
-        <v>153</v>
+        <f t="shared" si="4"/>
+        <v>76.500000012853619</v>
       </c>
       <c r="B155">
         <v>1.335176878</v>
@@ -6511,13 +6665,14 @@
         <v>9.0915067860000001</v>
       </c>
       <c r="D155">
-        <f t="shared" si="2"/>
-        <v>9.0740149708454627</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.2125970436666447</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A156">
-        <v>154</v>
+        <f t="shared" si="4"/>
+        <v>76.999999997958327</v>
       </c>
       <c r="B156">
         <v>1.3439035239999999</v>
@@ -6526,13 +6681,14 @@
         <v>9.0873577280000006</v>
       </c>
       <c r="D156">
-        <f t="shared" si="2"/>
-        <v>9.0629547450216723</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.2467949535224574</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A157">
-        <v>155</v>
+        <f t="shared" si="4"/>
+        <v>77.499999983063063</v>
       </c>
       <c r="B157">
         <v>1.3526301700000001</v>
@@ -6541,13 +6697,14 @@
         <v>9.0823237670000001</v>
       </c>
       <c r="D157">
-        <f t="shared" si="2"/>
-        <v>9.0499478417447534</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.2810732511993912</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A158">
-        <v>156</v>
+        <f t="shared" si="4"/>
+        <v>78.000000025463564</v>
       </c>
       <c r="B158">
         <v>1.3613568170000001</v>
@@ -6556,13 +6713,14 @@
         <v>9.0764125159999995</v>
       </c>
       <c r="D158">
-        <f t="shared" si="2"/>
-        <v>9.0349998697601208</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.3154298261920832</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A159">
-        <v>157</v>
+        <f t="shared" si="4"/>
+        <v>78.500000010568286</v>
       </c>
       <c r="B159">
         <v>1.3700834630000001</v>
@@ -6571,13 +6729,14 @@
         <v>9.0696316350000004</v>
       </c>
       <c r="D159">
-        <f t="shared" si="2"/>
-        <v>9.0181172803489602</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.3498625513513729</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A160">
-        <v>158</v>
+        <f t="shared" si="4"/>
+        <v>78.999999995673008</v>
       </c>
       <c r="B160">
         <v>1.378810109</v>
@@ -6586,13 +6745,14 @@
         <v>9.0619888290000006</v>
       </c>
       <c r="D160">
-        <f t="shared" si="2"/>
-        <v>8.9993073542683675</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.3843693066372378</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A161">
-        <v>159</v>
+        <f t="shared" si="4"/>
+        <v>79.49999998077773</v>
       </c>
       <c r="B161">
         <v>1.387536755</v>
@@ -6601,13 +6761,14 @@
         <v>9.053491846</v>
       </c>
       <c r="D161">
-        <f t="shared" si="2"/>
-        <v>8.9785782052400691</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.418947963510595</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A162">
-        <v>160</v>
+        <f t="shared" si="4"/>
+        <v>80.000000023178231</v>
       </c>
       <c r="B162">
         <v>1.396263402</v>
@@ -6616,13 +6777,14 @@
         <v>9.0441484780000003</v>
       </c>
       <c r="D162">
-        <f t="shared" si="2"/>
-        <v>8.955938772145382</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.4535963929714715</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A163">
-        <v>161</v>
+        <f t="shared" si="4"/>
+        <v>80.500000008282939</v>
       </c>
       <c r="B163">
         <v>1.4049900479999999</v>
@@ -6631,13 +6793,14 @@
         <v>9.0339665500000006</v>
       </c>
       <c r="D163">
-        <f t="shared" si="2"/>
-        <v>8.9313988257645178</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.4883124498008606</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A164">
-        <v>162</v>
+        <f t="shared" si="4"/>
+        <v>80.999999993387675</v>
       </c>
       <c r="B164">
         <v>1.4137166940000001</v>
@@ -6646,13 +6809,14 @@
         <v>9.0229539269999997</v>
       </c>
       <c r="D164">
-        <f t="shared" si="2"/>
-        <v>8.9049689489967605</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.5230939965154393</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A165">
-        <v>163</v>
+        <f t="shared" si="4"/>
+        <v>81.499999978492397</v>
       </c>
       <c r="B165">
         <v>1.4224433400000001</v>
@@ -6661,13 +6825,14 @@
         <v>9.0111185089999992</v>
       </c>
       <c r="D165">
-        <f t="shared" si="2"/>
-        <v>8.8766605424539335</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.5579388876256979</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A166">
-        <v>164</v>
+        <f t="shared" si="4"/>
+        <v>82.000000020892898</v>
       </c>
       <c r="B166">
         <v>1.4311699870000001</v>
@@ -6676,13 +6841,14 @@
         <v>8.9984682239999998</v>
       </c>
       <c r="D166">
-        <f t="shared" si="2"/>
-        <v>8.846485813493457</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.5928449777381131</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A167">
-        <v>165</v>
+        <f t="shared" si="4"/>
+        <v>82.50000000599762</v>
       </c>
       <c r="B167">
         <v>1.439896633</v>
@@ -6691,13 +6857,14 @@
         <v>8.9850110339999993</v>
       </c>
       <c r="D167">
-        <f t="shared" si="2"/>
-        <v>8.814457784996403</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.6278101056809096</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A168">
-        <v>166</v>
+        <f t="shared" si="4"/>
+        <v>82.999999991102342</v>
       </c>
       <c r="B168">
         <v>1.448623279</v>
@@ -6706,13 +6873,14 @@
         <v>8.9707549259999997</v>
       </c>
       <c r="D168">
-        <f t="shared" si="2"/>
-        <v>8.7805902690041506</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.6628321186369002</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A169">
-        <v>167</v>
+        <f t="shared" si="4"/>
+        <v>83.49999997620705</v>
       </c>
       <c r="B169">
         <v>1.4573499249999999</v>
@@ -6721,13 +6889,14 @@
         <v>8.9557079149999996</v>
       </c>
       <c r="D169">
-        <f t="shared" si="2"/>
-        <v>8.7448978743779691</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.6979088562834859</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A170">
-        <v>168</v>
+        <f t="shared" si="4"/>
+        <v>84.000000018607565</v>
       </c>
       <c r="B170">
         <v>1.466076572</v>
@@ -6736,13 +6905,14 @@
         <v>8.9398780379999998</v>
       </c>
       <c r="D170">
-        <f t="shared" si="2"/>
-        <v>8.7073959927458873</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.7330381589508428</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A171">
-        <v>169</v>
+        <f t="shared" si="4"/>
+        <v>84.500000003712273</v>
       </c>
       <c r="B171">
         <v>1.4748032179999999</v>
@@ -6751,13 +6921,14 @@
         <v>8.9232733549999992</v>
       </c>
       <c r="D171">
-        <f t="shared" si="2"/>
-        <v>8.6681008092588989</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.7682178516472353</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A172">
-        <v>170</v>
+        <f t="shared" si="4"/>
+        <v>84.999999988817009</v>
       </c>
       <c r="B172">
         <v>1.4835298640000001</v>
@@ -6766,13 +6937,14 @@
         <v>8.9059019450000001</v>
       </c>
       <c r="D172">
-        <f t="shared" si="2"/>
-        <v>8.6270292698259681</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.8034457683461893</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A173">
-        <v>171</v>
+        <f t="shared" si="4"/>
+        <v>85.499999973921732</v>
       </c>
       <c r="B173">
         <v>1.49225651</v>
@@ -6781,13 +6953,14 @@
         <v>8.8877719059999993</v>
       </c>
       <c r="D173">
-        <f t="shared" si="2"/>
-        <v>8.5841990907868961</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.8387197360239904</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A174">
-        <v>172</v>
+        <f t="shared" si="4"/>
+        <v>86.000000016322232</v>
       </c>
       <c r="B174">
         <v>1.5009831570000001</v>
@@ -6796,13 +6969,14 @@
         <v>8.8688913520000003</v>
       </c>
       <c r="D174">
-        <f t="shared" si="2"/>
-        <v>8.5396287418699419</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.8740375828658475</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A175">
-        <v>173</v>
+        <f t="shared" si="4"/>
+        <v>86.500000001426955</v>
       </c>
       <c r="B175">
         <v>1.509709803</v>
@@ -6811,13 +6985,14 @@
         <v>8.8492684110000006</v>
       </c>
       <c r="D175">
-        <f t="shared" si="2"/>
-        <v>8.4933374588519648</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.9093971222065216</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A176">
-        <v>174</v>
+        <f t="shared" si="4"/>
+        <v>86.999999986531662</v>
       </c>
       <c r="B176">
         <v>1.518436449</v>
@@ -6826,13 +7001,14 @@
         <v>8.8289112250000006</v>
       </c>
       <c r="D176">
-        <f t="shared" si="2"/>
-        <v>8.4453452046178032</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.9447961769478512</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A177">
-        <v>175</v>
+        <f t="shared" si="4"/>
+        <v>87.499999971636385</v>
       </c>
       <c r="B177">
         <v>1.5271630949999999</v>
@@ -6841,13 +7017,14 @@
         <v>8.8078279439999996</v>
       </c>
       <c r="D177">
-        <f t="shared" si="2"/>
-        <v>8.3956726807797111</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>3.9802325635095284</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A178">
-        <v>176</v>
+        <f t="shared" si="4"/>
+        <v>88.000000014036885</v>
       </c>
       <c r="B178">
         <v>1.5358897419999999</v>
@@ -6856,13 +7033,14 @@
         <v>8.7860267309999998</v>
       </c>
       <c r="D178">
-        <f t="shared" si="2"/>
-        <v>8.3443413077632549</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>4.0157041000751068</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A179">
-        <v>177</v>
+        <f t="shared" si="4"/>
+        <v>88.499999999141608</v>
       </c>
       <c r="B179">
         <v>1.5446163879999999</v>
@@ -6871,13 +7049,14 @@
         <v>8.7635157540000002</v>
       </c>
       <c r="D179">
-        <f t="shared" si="2"/>
-        <v>8.2913732392841091</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>4.0512085904638209</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A180">
-        <v>178</v>
+        <f t="shared" si="4"/>
+        <v>88.999999984246344</v>
       </c>
       <c r="B180">
         <v>1.5533430340000001</v>
@@ -6886,13 +7065,14 @@
         <v>8.7403031880000004</v>
       </c>
       <c r="D180">
-        <f t="shared" si="2"/>
-        <v>8.2367913175003871</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>4.0867438486543604</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A181">
-        <v>179</v>
+        <f t="shared" si="4"/>
+        <v>89.500000026646845</v>
       </c>
       <c r="B181">
         <v>1.5620696810000001</v>
@@ -6901,13 +7081,14 @@
         <v>8.7163972140000006</v>
       </c>
       <c r="D181">
-        <f t="shared" si="2"/>
-        <v>8.1806190799714393</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>4.1223076867416104</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A182">
-        <v>180</v>
+        <f t="shared" si="4"/>
+        <v>90.000000011751567</v>
       </c>
       <c r="B182">
         <v>1.570796327</v>
@@ -6916,8 +7097,8 @@
         <v>8.6918060130000008</v>
       </c>
       <c r="D182">
-        <f t="shared" si="2"/>
-        <v>8.1228807696447198</v>
+        <f t="shared" si="5"/>
+        <v>4.1578979028300624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>